<commit_message>
12/35 searching question done
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AbhishekBiswas\Desktop\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CF230C6-CBAB-48FB-B10F-1B492E858A87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BD63C75-CAB9-4446-B8C7-CA183C9C2705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Arrays" sheetId="1" r:id="rId1"/>
+    <sheet name="Searching" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="143">
   <si>
     <t xml:space="preserve">DSA </t>
   </si>
@@ -350,18 +351,124 @@
   </si>
   <si>
     <t>Check if array is sorted and rotated</t>
+  </si>
+  <si>
+    <t>Binary Search (Iterative)</t>
+  </si>
+  <si>
+    <t>Binary Search (Recursive)</t>
+  </si>
+  <si>
+    <t>Index of first Occurrence in Sorted</t>
+  </si>
+  <si>
+    <t>Index of last Occurrence in Sorted</t>
+  </si>
+  <si>
+    <t>Count Occurrences in Sorted</t>
+  </si>
+  <si>
+    <t>Count 1s in a Sorted Binary Array</t>
+  </si>
+  <si>
+    <t>Square root</t>
+  </si>
+  <si>
+    <t>Search in Infinite Sized Array</t>
+  </si>
+  <si>
+    <t>Search in Sorted Rotated Array</t>
+  </si>
+  <si>
+    <t>Find a Peak Element</t>
+  </si>
+  <si>
+    <t>Two Pointers Approach</t>
+  </si>
+  <si>
+    <t>Triplet in a Sorted Array</t>
+  </si>
+  <si>
+    <t>Median of two sorted arrays</t>
+  </si>
+  <si>
+    <t>Repeating Elements Part (1)</t>
+  </si>
+  <si>
+    <t>Repeating Elements Part (2)</t>
+  </si>
+  <si>
+    <t>Allocate Minimum Pages (Naive Method)</t>
+  </si>
+  <si>
+    <t>Allocate Minimum Pages (Binary Search)</t>
+  </si>
+  <si>
+    <t>Search an Element in an array</t>
+  </si>
+  <si>
+    <t>Searching an element in a sorted array</t>
+  </si>
+  <si>
+    <t>Floor in a Sorted Array</t>
+  </si>
+  <si>
+    <t>Maximum Water Between Two Buildings</t>
+  </si>
+  <si>
+    <t>Allocate minimum number of pages</t>
+  </si>
+  <si>
+    <t>Two Repeated Elements</t>
+  </si>
+  <si>
+    <t>Count only Repeated</t>
+  </si>
+  <si>
+    <t>Median of Two sorted arrays</t>
+  </si>
+  <si>
+    <t>Find Indexes of a subarray with given sum</t>
+  </si>
+  <si>
+    <t>Roof Top</t>
+  </si>
+  <si>
+    <t>Peak element</t>
+  </si>
+  <si>
+    <t>Minimum Number in a sorted rotated array</t>
+  </si>
+  <si>
+    <t>Square root of a number</t>
+  </si>
+  <si>
+    <t>Count 1's in binary array</t>
+  </si>
+  <si>
+    <t>Count More than n/k Occurences</t>
+  </si>
+  <si>
+    <t>Left Index</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -392,8 +499,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF0F2B3C"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF090C10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -418,8 +555,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -428,102 +571,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color auto="1"/>
+      <left style="thin">
+        <color indexed="64"/>
       </left>
-      <right/>
-      <top style="medium">
-        <color auto="1"/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -531,33 +589,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -835,13 +894,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="111" zoomScaleNormal="111" workbookViewId="0">
-      <selection activeCell="C65" sqref="C65"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="111" zoomScaleNormal="111" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25:C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="29.77734375" customWidth="1"/>
+    <col min="1" max="1" width="23.5546875" customWidth="1"/>
     <col min="2" max="2" width="53.5546875" customWidth="1"/>
     <col min="4" max="4" width="18.109375" customWidth="1"/>
   </cols>
@@ -868,586 +927,586 @@
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="4"/>
+      <c r="C16" s="8"/>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="10"/>
+      <c r="C17" s="8"/>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="7"/>
+      <c r="C24" s="8"/>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C25" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="14" t="s">
+      <c r="A26" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B26" s="15" t="s">
+      <c r="B26" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C26" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C27" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="C28" s="7" t="s">
+      <c r="C28" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="C29" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="1" t="s">
+      <c r="A30" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="B30" s="16" t="s">
+      <c r="B30" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="C30" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="1" t="s">
+      <c r="A31" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="B31" s="17" t="s">
+      <c r="B31" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="C31" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B32" s="16" t="s">
+      <c r="B32" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="C32" s="7" t="s">
+      <c r="C32" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="1" t="s">
+      <c r="A33" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="B33" s="16" t="s">
+      <c r="B33" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="C33" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="1" t="s">
+      <c r="A34" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="B34" s="16" t="s">
+      <c r="B34" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="C34" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="1" t="s">
+      <c r="A35" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="B35" s="16" t="s">
+      <c r="B35" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="C35" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="1" t="s">
+      <c r="A36" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="B36" s="18" t="s">
+      <c r="B36" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="C36" s="1"/>
+      <c r="C36" s="8"/>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" s="1" t="s">
+      <c r="A37" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="B37" s="16" t="s">
+      <c r="B37" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C37" s="8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38" s="1" t="s">
+      <c r="A38" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B38" s="16" t="s">
+      <c r="B38" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C38" s="8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="39" spans="1:3">
-      <c r="A39" s="1" t="s">
+      <c r="A39" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="B39" s="16" t="s">
+      <c r="B39" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C39" s="8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:3">
-      <c r="A40" s="1" t="s">
+      <c r="A40" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="B40" s="16" t="s">
+      <c r="B40" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C40" s="8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="41" spans="1:3">
-      <c r="A41" s="1" t="s">
+      <c r="A41" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="B41" s="16" t="s">
+      <c r="B41" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C41" s="8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="42" spans="1:3">
-      <c r="A42" s="1" t="s">
+      <c r="A42" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="B42" s="16" t="s">
+      <c r="B42" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C42" s="8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="43" spans="1:3">
-      <c r="A43" s="1" t="s">
+      <c r="A43" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="B43" s="16" t="s">
+      <c r="B43" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C43" s="8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="44" spans="1:3">
-      <c r="A44" s="1" t="s">
+      <c r="A44" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="B44" s="16" t="s">
+      <c r="B44" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C44" s="8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="45" spans="1:3">
-      <c r="A45" s="1" t="s">
+      <c r="A45" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="B45" s="16" t="s">
+      <c r="B45" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C45" s="8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="46" spans="1:3">
-      <c r="A46" s="1" t="s">
+      <c r="A46" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="B46" s="16" t="s">
+      <c r="B46" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C46" s="8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="47" spans="1:3">
-      <c r="A47" s="1" t="s">
+      <c r="A47" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="B47" s="16" t="s">
+      <c r="B47" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C47" s="8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="48" spans="1:3">
-      <c r="A48" s="1" t="s">
+      <c r="A48" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="B48" s="16" t="s">
+      <c r="B48" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C48" s="8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="49" spans="1:3">
-      <c r="A49" s="1" t="s">
+      <c r="A49" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="B49" s="18" t="s">
+      <c r="B49" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="C49" s="1"/>
+      <c r="C49" s="8"/>
     </row>
     <row r="50" spans="1:3">
-      <c r="A50" s="1" t="s">
+      <c r="A50" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="B50" s="16" t="s">
+      <c r="B50" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="C50" s="19" t="s">
+      <c r="C50" s="16" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="1" t="s">
+      <c r="A51" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="B51" s="16" t="s">
+      <c r="B51" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C51" s="8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="52" spans="1:3">
-      <c r="A52" s="1" t="s">
+      <c r="A52" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="B52" s="16" t="s">
+      <c r="B52" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C52" s="8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="53" spans="1:3">
-      <c r="A53" s="1" t="s">
+      <c r="A53" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="B53" s="16" t="s">
+      <c r="B53" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C53" s="8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="54" spans="1:3">
-      <c r="A54" s="1" t="s">
+      <c r="A54" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="B54" s="16" t="s">
+      <c r="B54" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="C54" s="8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="55" spans="1:3">
-      <c r="A55" s="1" t="s">
+      <c r="A55" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="B55" s="16" t="s">
+      <c r="B55" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C55" s="8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="56" spans="1:3">
-      <c r="A56" s="1" t="s">
+      <c r="A56" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="B56" s="16" t="s">
+      <c r="B56" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="C56" s="8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="57" spans="1:3">
-      <c r="A57" s="1" t="s">
+      <c r="A57" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="B57" s="16" t="s">
+      <c r="B57" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="C57" s="8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="58" spans="1:3">
-      <c r="A58" s="1" t="s">
+      <c r="A58" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="B58" s="16" t="s">
+      <c r="B58" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C58" s="8" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1458,4 +1517,357 @@
     <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Confidential</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{800E1D52-B823-4FB2-8C01-6293B0B5F1C7}">
+  <dimension ref="A3:C38"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="19.5546875" customWidth="1"/>
+    <col min="2" max="2" width="43.6640625" customWidth="1"/>
+    <col min="3" max="3" width="20.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.6">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.6">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.6">
+      <c r="A6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.6">
+      <c r="A7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C7" s="6"/>
+    </row>
+    <row r="8" spans="1:3" ht="15.6">
+      <c r="A8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C8" s="6"/>
+    </row>
+    <row r="9" spans="1:3" ht="15.6">
+      <c r="A9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C9" s="6"/>
+    </row>
+    <row r="10" spans="1:3" ht="15.6">
+      <c r="A10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C10" s="6"/>
+    </row>
+    <row r="11" spans="1:3" ht="15.6">
+      <c r="A11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C11" s="6"/>
+    </row>
+    <row r="12" spans="1:3" ht="15.6">
+      <c r="A12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C12" s="6"/>
+    </row>
+    <row r="13" spans="1:3" ht="15.6">
+      <c r="A13" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C13" s="6"/>
+    </row>
+    <row r="14" spans="1:3" ht="15.6">
+      <c r="A14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C14" s="6"/>
+    </row>
+    <row r="15" spans="1:3" ht="15.6">
+      <c r="A15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C15" s="6"/>
+    </row>
+    <row r="16" spans="1:3" ht="15.6">
+      <c r="A16" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C16" s="6"/>
+    </row>
+    <row r="17" spans="1:3" ht="15.6">
+      <c r="A17" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C17" s="6"/>
+    </row>
+    <row r="18" spans="1:3" ht="15.6">
+      <c r="A18" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C18" s="6"/>
+    </row>
+    <row r="19" spans="1:3" ht="15.6">
+      <c r="A19" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C19" s="6"/>
+    </row>
+    <row r="20" spans="1:3" ht="15.6">
+      <c r="A20" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C20" s="6"/>
+    </row>
+    <row r="21" spans="1:3" ht="15.6">
+      <c r="A21" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="C21" s="6"/>
+    </row>
+    <row r="22" spans="1:3" ht="15.6">
+      <c r="A22" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="C22" s="6"/>
+    </row>
+    <row r="23" spans="1:3" ht="15.6">
+      <c r="A23" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="C23" s="6"/>
+    </row>
+    <row r="24" spans="1:3" ht="15.6">
+      <c r="A24" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="C24" s="6"/>
+    </row>
+    <row r="25" spans="1:3" ht="15.6">
+      <c r="A25" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="C25" s="6"/>
+    </row>
+    <row r="26" spans="1:3" ht="15.6">
+      <c r="A26" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="C26" s="6"/>
+    </row>
+    <row r="27" spans="1:3" ht="15.6">
+      <c r="A27" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="C27" s="6"/>
+    </row>
+    <row r="28" spans="1:3" ht="15.6">
+      <c r="A28" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="C28" s="6"/>
+    </row>
+    <row r="29" spans="1:3" ht="15.6">
+      <c r="A29" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C29" s="6"/>
+    </row>
+    <row r="30" spans="1:3" ht="15.6">
+      <c r="A30" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="C30" s="6"/>
+    </row>
+    <row r="31" spans="1:3" ht="15.6">
+      <c r="A31" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="C31" s="6"/>
+    </row>
+    <row r="32" spans="1:3" ht="15.6">
+      <c r="A32" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="C32" s="6"/>
+    </row>
+    <row r="33" spans="1:3" ht="15.6">
+      <c r="A33" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="C33" s="6"/>
+    </row>
+    <row r="34" spans="1:3" ht="15.6">
+      <c r="A34" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C34" s="6"/>
+    </row>
+    <row r="35" spans="1:3" ht="15.6">
+      <c r="A35" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="C35" s="6"/>
+    </row>
+    <row r="36" spans="1:3" ht="15.6">
+      <c r="A36" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="C36" s="6"/>
+    </row>
+    <row r="37" spans="1:3" ht="15.6">
+      <c r="A37" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="C37" s="6"/>
+    </row>
+    <row r="38" spans="1:3" ht="15.6">
+      <c r="A38" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C38" s="6"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="9" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Recursion Added && Math Added
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AbhishekBiswas\Desktop\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E0E3E71-8959-4319-82BB-369B860938C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{612CE840-8F80-4B7A-AF2D-372C9D29FCC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arrays" sheetId="1" r:id="rId1"/>
@@ -18,8 +18,8 @@
     <sheet name="Sorting" sheetId="3" r:id="rId3"/>
     <sheet name="Matrix" sheetId="4" r:id="rId4"/>
     <sheet name="Maths" sheetId="7" r:id="rId5"/>
-    <sheet name="Bit magic" sheetId="6" r:id="rId6"/>
-    <sheet name="Recursion" sheetId="8" r:id="rId7"/>
+    <sheet name="Recursion" sheetId="8" r:id="rId6"/>
+    <sheet name="Bit magic" sheetId="6" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Matrix!$A$5:$C$29</definedName>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="267">
   <si>
     <t xml:space="preserve">DSA </t>
   </si>
@@ -1062,7 +1062,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1097,14 +1097,10 @@
     <xf numFmtId="0" fontId="18" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1129,6 +1125,17 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1777,7 +1784,7 @@
       <c r="A36" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="B36" s="34" t="s">
+      <c r="B36" s="32" t="s">
         <v>69</v>
       </c>
       <c r="C36" s="17"/>
@@ -1918,7 +1925,7 @@
       <c r="A49" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="B49" s="34" t="s">
+      <c r="B49" s="32" t="s">
         <v>92</v>
       </c>
       <c r="C49" s="17"/>
@@ -1930,7 +1937,7 @@
       <c r="B50" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="C50" s="33" t="s">
+      <c r="C50" s="31" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2036,7 +2043,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{800E1D52-B823-4FB2-8C01-6293B0B5F1C7}">
   <dimension ref="A3:C38"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -2098,7 +2105,7 @@
       <c r="B7" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="C7" s="39" t="s">
+      <c r="C7" s="37" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2109,7 +2116,7 @@
       <c r="B8" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="C8" s="39" t="s">
+      <c r="C8" s="37" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2120,7 +2127,7 @@
       <c r="B9" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="C9" s="39" t="s">
+      <c r="C9" s="37" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2131,7 +2138,7 @@
       <c r="B10" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="C10" s="39" t="s">
+      <c r="C10" s="37" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2142,7 +2149,7 @@
       <c r="B11" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="C11" s="39" t="s">
+      <c r="C11" s="37" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2153,7 +2160,7 @@
       <c r="B12" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C12" s="39" t="s">
+      <c r="C12" s="37" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2164,7 +2171,7 @@
       <c r="B13" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="C13" s="39" t="s">
+      <c r="C13" s="37" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2175,7 +2182,7 @@
       <c r="B14" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="C14" s="39" t="s">
+      <c r="C14" s="37" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2186,54 +2193,54 @@
       <c r="B15" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="C15" s="39" t="s">
+      <c r="C15" s="37" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.6">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="36" t="s">
+      <c r="B16" s="34" t="s">
         <v>122</v>
       </c>
-      <c r="C16" s="37"/>
+      <c r="C16" s="35"/>
     </row>
     <row r="17" spans="1:3" ht="15.6">
-      <c r="A17" s="35" t="s">
+      <c r="A17" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="36" t="s">
+      <c r="B17" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="C17" s="37"/>
+      <c r="C17" s="35"/>
     </row>
     <row r="18" spans="1:3" ht="15.6">
-      <c r="A18" s="35" t="s">
+      <c r="A18" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="36" t="s">
+      <c r="B18" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="C18" s="37"/>
+      <c r="C18" s="35"/>
     </row>
     <row r="19" spans="1:3" ht="15.6">
-      <c r="A19" s="35" t="s">
+      <c r="A19" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="36" t="s">
+      <c r="B19" s="34" t="s">
         <v>125</v>
       </c>
-      <c r="C19" s="37"/>
+      <c r="C19" s="35"/>
     </row>
     <row r="20" spans="1:3" ht="15.6">
-      <c r="A20" s="35" t="s">
+      <c r="A20" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="36" t="s">
+      <c r="B20" s="34" t="s">
         <v>126</v>
       </c>
-      <c r="C20" s="37"/>
+      <c r="C20" s="35"/>
     </row>
     <row r="21" spans="1:3" ht="15.6">
       <c r="A21" s="2" t="s">
@@ -2242,7 +2249,7 @@
       <c r="B21" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="C21" s="39" t="s">
+      <c r="C21" s="37" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2253,7 +2260,7 @@
       <c r="B22" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="C22" s="39" t="s">
+      <c r="C22" s="37" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2264,27 +2271,27 @@
       <c r="B23" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="C23" s="39" t="s">
+      <c r="C23" s="37" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15.6">
-      <c r="A24" s="35" t="s">
+      <c r="A24" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="38" t="s">
+      <c r="B24" s="36" t="s">
         <v>130</v>
       </c>
-      <c r="C24" s="37"/>
+      <c r="C24" s="35"/>
     </row>
     <row r="25" spans="1:3" ht="15.6">
-      <c r="A25" s="35" t="s">
+      <c r="A25" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="38" t="s">
+      <c r="B25" s="36" t="s">
         <v>131</v>
       </c>
-      <c r="C25" s="37"/>
+      <c r="C25" s="35"/>
     </row>
     <row r="26" spans="1:3" ht="15.6">
       <c r="A26" s="2" t="s">
@@ -2293,7 +2300,7 @@
       <c r="B26" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="C26" s="39" t="s">
+      <c r="C26" s="37" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2304,27 +2311,27 @@
       <c r="B27" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="C27" s="39" t="s">
+      <c r="C27" s="37" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15.6">
-      <c r="A28" s="35" t="s">
+      <c r="A28" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="B28" s="38" t="s">
+      <c r="B28" s="36" t="s">
         <v>134</v>
       </c>
-      <c r="C28" s="37"/>
+      <c r="C28" s="35"/>
     </row>
     <row r="29" spans="1:3" ht="15.6">
-      <c r="A29" s="35" t="s">
+      <c r="A29" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="B29" s="38" t="s">
+      <c r="B29" s="36" t="s">
         <v>135</v>
       </c>
-      <c r="C29" s="37"/>
+      <c r="C29" s="35"/>
     </row>
     <row r="30" spans="1:3" ht="15.6">
       <c r="A30" s="2" t="s">
@@ -2333,7 +2340,7 @@
       <c r="B30" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="C30" s="39" t="s">
+      <c r="C30" s="37" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2344,18 +2351,18 @@
       <c r="B31" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="C31" s="39" t="s">
+      <c r="C31" s="37" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="15.6">
-      <c r="A32" s="35" t="s">
+      <c r="A32" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="B32" s="38" t="s">
+      <c r="B32" s="36" t="s">
         <v>138</v>
       </c>
-      <c r="C32" s="37"/>
+      <c r="C32" s="35"/>
     </row>
     <row r="33" spans="1:3" ht="15.6">
       <c r="A33" s="2" t="s">
@@ -2364,18 +2371,18 @@
       <c r="B33" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="C33" s="39" t="s">
+      <c r="C33" s="37" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="15.6">
-      <c r="A34" s="35" t="s">
+      <c r="A34" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="B34" s="38" t="s">
+      <c r="B34" s="36" t="s">
         <v>97</v>
       </c>
-      <c r="C34" s="37"/>
+      <c r="C34" s="35"/>
     </row>
     <row r="35" spans="1:3" ht="15.6">
       <c r="A35" s="2" t="s">
@@ -2384,18 +2391,18 @@
       <c r="B35" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="C35" s="39" t="s">
+      <c r="C35" s="37" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="15.6">
-      <c r="A36" s="35" t="s">
+      <c r="A36" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="B36" s="38" t="s">
+      <c r="B36" s="36" t="s">
         <v>141</v>
       </c>
-      <c r="C36" s="37"/>
+      <c r="C36" s="35"/>
     </row>
     <row r="37" spans="1:3" ht="15.6">
       <c r="A37" s="2" t="s">
@@ -2404,7 +2411,7 @@
       <c r="B37" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="C37" s="39" t="s">
+      <c r="C37" s="37" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2415,7 +2422,7 @@
       <c r="B38" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C38" s="39" t="s">
+      <c r="C38" s="37" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2429,7 +2436,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90C4FD7F-5EC5-490A-B30F-D01CABD8A4B4}">
   <dimension ref="A4:E60"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
@@ -2640,34 +2647,34 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="15.6">
-      <c r="A22" s="40" t="s">
+      <c r="A22" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="36" t="s">
+      <c r="B22" s="34" t="s">
         <v>160</v>
       </c>
-      <c r="C22" s="40"/>
+      <c r="C22" s="38"/>
       <c r="E22" s="10">
         <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15.6">
-      <c r="A23" s="40" t="s">
+      <c r="A23" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="36" t="s">
+      <c r="B23" s="34" t="s">
         <v>161</v>
       </c>
-      <c r="C23" s="40"/>
+      <c r="C23" s="38"/>
     </row>
     <row r="24" spans="1:5" ht="15.6">
-      <c r="A24" s="40" t="s">
+      <c r="A24" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="B24" s="36" t="s">
+      <c r="B24" s="34" t="s">
         <v>162</v>
       </c>
-      <c r="C24" s="40"/>
+      <c r="C24" s="38"/>
     </row>
     <row r="25" spans="1:5" ht="15.6">
       <c r="A25" s="11" t="s">
@@ -2703,13 +2710,13 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="15.6">
-      <c r="A28" s="40" t="s">
+      <c r="A28" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="B28" s="36" t="s">
+      <c r="B28" s="34" t="s">
         <v>166</v>
       </c>
-      <c r="C28" s="40"/>
+      <c r="C28" s="38"/>
     </row>
     <row r="29" spans="1:5" ht="15.6">
       <c r="A29" s="11" t="s">
@@ -2734,67 +2741,67 @@
       </c>
     </row>
     <row r="31" spans="1:5" ht="15.6">
-      <c r="A31" s="40" t="s">
+      <c r="A31" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="B31" s="36" t="s">
+      <c r="B31" s="34" t="s">
         <v>169</v>
       </c>
-      <c r="C31" s="40"/>
+      <c r="C31" s="38"/>
     </row>
     <row r="32" spans="1:5" ht="15.6">
-      <c r="A32" s="40" t="s">
+      <c r="A32" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="B32" s="36" t="s">
+      <c r="B32" s="34" t="s">
         <v>170</v>
       </c>
-      <c r="C32" s="40"/>
+      <c r="C32" s="38"/>
     </row>
     <row r="33" spans="1:3" ht="15.6">
-      <c r="A33" s="40" t="s">
+      <c r="A33" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="B33" s="36" t="s">
+      <c r="B33" s="34" t="s">
         <v>171</v>
       </c>
-      <c r="C33" s="40"/>
+      <c r="C33" s="38"/>
     </row>
     <row r="34" spans="1:3" ht="15.6">
-      <c r="A34" s="40" t="s">
+      <c r="A34" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="B34" s="36" t="s">
+      <c r="B34" s="34" t="s">
         <v>172</v>
       </c>
-      <c r="C34" s="40"/>
+      <c r="C34" s="38"/>
     </row>
     <row r="35" spans="1:3" ht="15.6">
-      <c r="A35" s="40" t="s">
+      <c r="A35" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="B35" s="36" t="s">
+      <c r="B35" s="34" t="s">
         <v>173</v>
       </c>
-      <c r="C35" s="40"/>
+      <c r="C35" s="38"/>
     </row>
     <row r="36" spans="1:3" ht="15.6">
-      <c r="A36" s="40" t="s">
+      <c r="A36" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="B36" s="36" t="s">
+      <c r="B36" s="34" t="s">
         <v>174</v>
       </c>
-      <c r="C36" s="40"/>
+      <c r="C36" s="38"/>
     </row>
     <row r="37" spans="1:3" ht="15.6">
-      <c r="A37" s="40" t="s">
+      <c r="A37" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="B37" s="36" t="s">
+      <c r="B37" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="C37" s="40"/>
+      <c r="C37" s="38"/>
     </row>
     <row r="38" spans="1:3" ht="15.6">
       <c r="A38" s="11" t="s">
@@ -2819,40 +2826,40 @@
       </c>
     </row>
     <row r="40" spans="1:3" ht="15.6">
-      <c r="A40" s="40" t="s">
+      <c r="A40" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="B40" s="38" t="s">
+      <c r="B40" s="36" t="s">
         <v>176</v>
       </c>
-      <c r="C40" s="40"/>
+      <c r="C40" s="38"/>
     </row>
     <row r="41" spans="1:3" ht="15.6">
-      <c r="A41" s="40" t="s">
+      <c r="A41" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="B41" s="38" t="s">
+      <c r="B41" s="36" t="s">
         <v>177</v>
       </c>
-      <c r="C41" s="40"/>
+      <c r="C41" s="38"/>
     </row>
     <row r="42" spans="1:3" ht="15.6">
-      <c r="A42" s="40" t="s">
+      <c r="A42" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="B42" s="38" t="s">
+      <c r="B42" s="36" t="s">
         <v>178</v>
       </c>
-      <c r="C42" s="40"/>
+      <c r="C42" s="38"/>
     </row>
     <row r="43" spans="1:3" ht="15.6">
-      <c r="A43" s="40" t="s">
+      <c r="A43" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="B43" s="38" t="s">
+      <c r="B43" s="36" t="s">
         <v>179</v>
       </c>
-      <c r="C43" s="40"/>
+      <c r="C43" s="38"/>
     </row>
     <row r="44" spans="1:3" ht="15.6">
       <c r="A44" s="11" t="s">
@@ -2866,40 +2873,40 @@
       </c>
     </row>
     <row r="45" spans="1:3" ht="15.6">
-      <c r="A45" s="40" t="s">
+      <c r="A45" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="B45" s="38" t="s">
+      <c r="B45" s="36" t="s">
         <v>181</v>
       </c>
-      <c r="C45" s="40"/>
+      <c r="C45" s="38"/>
     </row>
     <row r="46" spans="1:3" ht="15.6">
-      <c r="A46" s="40" t="s">
+      <c r="A46" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="B46" s="38" t="s">
+      <c r="B46" s="36" t="s">
         <v>182</v>
       </c>
-      <c r="C46" s="40"/>
+      <c r="C46" s="38"/>
     </row>
     <row r="47" spans="1:3" ht="15.6">
-      <c r="A47" s="40" t="s">
+      <c r="A47" s="38" t="s">
         <v>89</v>
       </c>
-      <c r="B47" s="38" t="s">
+      <c r="B47" s="36" t="s">
         <v>173</v>
       </c>
-      <c r="C47" s="40"/>
+      <c r="C47" s="38"/>
     </row>
     <row r="48" spans="1:3" ht="15.6">
-      <c r="A48" s="40" t="s">
+      <c r="A48" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="B48" s="38" t="s">
+      <c r="B48" s="36" t="s">
         <v>183</v>
       </c>
-      <c r="C48" s="40"/>
+      <c r="C48" s="38"/>
     </row>
     <row r="49" spans="1:3" ht="15.6">
       <c r="A49" s="11" t="s">
@@ -2924,13 +2931,13 @@
       </c>
     </row>
     <row r="51" spans="1:3" ht="15.6">
-      <c r="A51" s="40" t="s">
+      <c r="A51" s="38" t="s">
         <v>95</v>
       </c>
-      <c r="B51" s="38" t="s">
+      <c r="B51" s="36" t="s">
         <v>165</v>
       </c>
-      <c r="C51" s="40"/>
+      <c r="C51" s="38"/>
     </row>
     <row r="52" spans="1:3" ht="15.6">
       <c r="A52" s="11" t="s">
@@ -2944,13 +2951,13 @@
       </c>
     </row>
     <row r="53" spans="1:3" ht="15.6">
-      <c r="A53" s="40" t="s">
+      <c r="A53" s="38" t="s">
         <v>98</v>
       </c>
-      <c r="B53" s="38" t="s">
+      <c r="B53" s="36" t="s">
         <v>187</v>
       </c>
-      <c r="C53" s="40"/>
+      <c r="C53" s="38"/>
     </row>
     <row r="54" spans="1:3" ht="15.6">
       <c r="A54" s="11" t="s">
@@ -3008,13 +3015,13 @@
       </c>
     </row>
     <row r="59" spans="1:3" ht="15.6">
-      <c r="A59" s="40" t="s">
+      <c r="A59" s="38" t="s">
         <v>192</v>
       </c>
-      <c r="B59" s="38" t="s">
+      <c r="B59" s="36" t="s">
         <v>176</v>
       </c>
-      <c r="C59" s="40"/>
+      <c r="C59" s="38"/>
     </row>
     <row r="60" spans="1:3" ht="15.6">
       <c r="A60" s="11" t="s">
@@ -3038,7 +3045,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05A54019-BCB4-4D3D-8A03-2417EABC3558}">
   <dimension ref="A5:C29"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -3064,16 +3071,16 @@
       <c r="A6" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="34" t="s">
         <v>194</v>
       </c>
-      <c r="C6" s="41"/>
+      <c r="C6" s="39"/>
     </row>
     <row r="7" spans="1:3" ht="15.6">
       <c r="A7" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="34" t="s">
         <v>195</v>
       </c>
       <c r="C7" s="16"/>
@@ -3148,7 +3155,7 @@
       <c r="A14" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="36" t="s">
+      <c r="B14" s="34" t="s">
         <v>201</v>
       </c>
       <c r="C14" s="16"/>
@@ -3243,7 +3250,7 @@
       <c r="A23" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="B23" s="38" t="s">
+      <c r="B23" s="36" t="s">
         <v>210</v>
       </c>
       <c r="C23" s="16"/>
@@ -3255,7 +3262,7 @@
       <c r="B24" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="C24" s="39" t="s">
+      <c r="C24" s="37" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3307,7 +3314,7 @@
       <c r="A29" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="B29" s="38" t="s">
+      <c r="B29" s="36" t="s">
         <v>216</v>
       </c>
       <c r="C29" s="16"/>
@@ -3323,16 +3330,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9345B1F2-0CB8-4135-96A4-D1912C3544D2}">
   <dimension ref="A5:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" style="24" customWidth="1"/>
-    <col min="2" max="2" width="45.21875" style="24" customWidth="1"/>
-    <col min="3" max="3" width="49" style="24" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="24"/>
+    <col min="1" max="1" width="31.88671875" style="23" customWidth="1"/>
+    <col min="2" max="2" width="45.21875" style="23" customWidth="1"/>
+    <col min="3" max="3" width="49" style="23" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="23"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:3">
@@ -3347,247 +3354,251 @@
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="24" t="s">
         <v>244</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="22" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="24" t="s">
         <v>245</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="22" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="24" t="s">
         <v>246</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="22" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="24" t="s">
         <v>247</v>
       </c>
-      <c r="C9" s="23" t="s">
+      <c r="C9" s="22" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="24" t="s">
         <v>248</v>
       </c>
-      <c r="C10" s="23" t="s">
+      <c r="C10" s="22" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="30" t="s">
+      <c r="A11" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="32" t="s">
+      <c r="B11" s="30" t="s">
         <v>249</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="22" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="30" t="s">
+      <c r="A12" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="30" t="s">
         <v>250</v>
       </c>
-      <c r="C12" s="23" t="s">
+      <c r="C12" s="22" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="26" t="s">
+      <c r="B13" s="30" t="s">
         <v>251</v>
       </c>
-      <c r="C13" s="22"/>
+      <c r="C13" s="28" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="22" t="s">
+      <c r="A14" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="26" t="s">
+      <c r="B14" s="45" t="s">
         <v>252</v>
       </c>
-      <c r="C14" s="22"/>
+      <c r="C14" s="44"/>
     </row>
     <row r="15" spans="1:3" ht="15" customHeight="1">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="27" t="s">
+      <c r="B15" s="43" t="s">
         <v>253</v>
       </c>
-      <c r="C15" s="22"/>
+      <c r="C15" s="28" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="30" t="s">
+      <c r="A16" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="32" t="s">
+      <c r="B16" s="30" t="s">
         <v>254</v>
       </c>
-      <c r="C16" s="30" t="s">
+      <c r="C16" s="28" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="30" t="s">
+      <c r="A17" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="32" t="s">
+      <c r="B17" s="30" t="s">
         <v>255</v>
       </c>
-      <c r="C17" s="30" t="s">
+      <c r="C17" s="28" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="19.2" customHeight="1">
-      <c r="A18" s="23" t="s">
+      <c r="A18" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="28" t="s">
+      <c r="B18" s="26" t="s">
         <v>256</v>
       </c>
-      <c r="C18" s="23" t="s">
+      <c r="C18" s="22" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="19.8" customHeight="1">
-      <c r="A19" s="23" t="s">
+      <c r="A19" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="28" t="s">
+      <c r="B19" s="26" t="s">
         <v>257</v>
       </c>
-      <c r="C19" s="23" t="s">
+      <c r="C19" s="22" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="17.399999999999999" customHeight="1">
-      <c r="A20" s="30" t="s">
+      <c r="A20" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="31" t="s">
+      <c r="B20" s="29" t="s">
         <v>258</v>
       </c>
-      <c r="C20" s="23" t="s">
+      <c r="C20" s="22" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="16.8" customHeight="1">
-      <c r="A21" s="23" t="s">
+      <c r="A21" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="28" t="s">
+      <c r="B21" s="26" t="s">
         <v>259</v>
       </c>
-      <c r="C21" s="23" t="s">
+      <c r="C21" s="22" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="23" t="s">
+      <c r="A22" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="28" t="s">
+      <c r="B22" s="26" t="s">
         <v>260</v>
       </c>
-      <c r="C22" s="23" t="s">
+      <c r="C22" s="22" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="22" t="s">
+      <c r="A23" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="B23" s="29" t="s">
+      <c r="B23" s="46" t="s">
         <v>261</v>
       </c>
-      <c r="C23" s="22"/>
+      <c r="C23" s="44"/>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="30" t="s">
+      <c r="A24" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="B24" s="31" t="s">
+      <c r="B24" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="C24" s="30" t="s">
+      <c r="C24" s="28" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="30" t="s">
+      <c r="A25" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="B25" s="31" t="s">
+      <c r="B25" s="29" t="s">
         <v>263</v>
       </c>
-      <c r="C25" s="23" t="s">
+      <c r="C25" s="22" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="30" t="s">
+      <c r="A26" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="B26" s="31" t="s">
+      <c r="B26" s="29" t="s">
         <v>264</v>
       </c>
-      <c r="C26" s="23" t="s">
+      <c r="C26" s="22" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="30" t="s">
+      <c r="A27" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="B27" s="31" t="s">
+      <c r="B27" s="29" t="s">
         <v>265</v>
       </c>
-      <c r="C27" s="23" t="s">
+      <c r="C27" s="22" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="30" t="s">
+      <c r="A28" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="B28" s="31" t="s">
+      <c r="B28" s="29" t="s">
         <v>266</v>
       </c>
-      <c r="C28" s="23" t="s">
+      <c r="C28" s="22" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3597,6 +3608,363 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46ACBD4C-1708-4E7B-88DE-7B19F26CFE31}">
+  <dimension ref="A5:C39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="21.5546875" style="40" customWidth="1"/>
+    <col min="2" max="2" width="70.44140625" style="40" customWidth="1"/>
+    <col min="3" max="3" width="45.77734375" style="40" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="40"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="1:3">
+      <c r="A5" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>217</v>
+      </c>
+      <c r="C6" s="41"/>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>218</v>
+      </c>
+      <c r="C7" s="41"/>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>219</v>
+      </c>
+      <c r="C8" s="41"/>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="C9" s="41"/>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>221</v>
+      </c>
+      <c r="C10" s="41"/>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>222</v>
+      </c>
+      <c r="C11" s="41"/>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="41" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="25" t="s">
+        <v>223</v>
+      </c>
+      <c r="C12" s="41"/>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="25" t="s">
+        <v>224</v>
+      </c>
+      <c r="C13" s="41"/>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="25" t="s">
+        <v>225</v>
+      </c>
+      <c r="C14" s="41"/>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>226</v>
+      </c>
+      <c r="C15" s="41"/>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="25" t="s">
+        <v>227</v>
+      </c>
+      <c r="C16" s="41"/>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="25" t="s">
+        <v>228</v>
+      </c>
+      <c r="C17" s="41"/>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="41" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="25" t="s">
+        <v>229</v>
+      </c>
+      <c r="C18" s="41"/>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="25" t="s">
+        <v>230</v>
+      </c>
+      <c r="C19" s="41"/>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="30" t="s">
+        <v>231</v>
+      </c>
+      <c r="C20" s="42" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="25" t="s">
+        <v>224</v>
+      </c>
+      <c r="C21" s="41"/>
+    </row>
+    <row r="22" spans="1:3" ht="15.6" customHeight="1">
+      <c r="A22" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="25" t="s">
+        <v>223</v>
+      </c>
+      <c r="C22" s="41"/>
+    </row>
+    <row r="23" spans="1:3" ht="13.8" hidden="1" customHeight="1">
+      <c r="A23" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="27" t="s">
+        <v>232</v>
+      </c>
+      <c r="C23" s="41"/>
+    </row>
+    <row r="24" spans="1:3" ht="18" hidden="1" customHeight="1">
+      <c r="A24" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="27" t="s">
+        <v>233</v>
+      </c>
+      <c r="C24" s="41"/>
+    </row>
+    <row r="25" spans="1:3" hidden="1">
+      <c r="A25" s="41" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="27" t="s">
+        <v>234</v>
+      </c>
+      <c r="C25" s="41"/>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" s="29" t="s">
+        <v>235</v>
+      </c>
+      <c r="C26" s="42" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="17.399999999999999" customHeight="1">
+      <c r="A27" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" s="29" t="s">
+        <v>236</v>
+      </c>
+      <c r="C27" s="42" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="16.8" customHeight="1">
+      <c r="A28" s="42" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" s="29" t="s">
+        <v>237</v>
+      </c>
+      <c r="C28" s="42" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="18" customHeight="1">
+      <c r="A29" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29" s="27" t="s">
+        <v>238</v>
+      </c>
+      <c r="C29" s="41"/>
+    </row>
+    <row r="30" spans="1:3" ht="18.600000000000001" customHeight="1">
+      <c r="A30" s="41" t="s">
+        <v>54</v>
+      </c>
+      <c r="B30" s="27" t="s">
+        <v>239</v>
+      </c>
+      <c r="C30" s="41"/>
+    </row>
+    <row r="31" spans="1:3" ht="15.6" customHeight="1">
+      <c r="A31" s="41" t="s">
+        <v>56</v>
+      </c>
+      <c r="B31" s="27" t="s">
+        <v>240</v>
+      </c>
+      <c r="C31" s="41"/>
+    </row>
+    <row r="32" spans="1:3" ht="16.8" customHeight="1">
+      <c r="A32" s="41" t="s">
+        <v>58</v>
+      </c>
+      <c r="B32" s="27" t="s">
+        <v>241</v>
+      </c>
+      <c r="C32" s="41"/>
+    </row>
+    <row r="33" spans="1:3" ht="15.6" customHeight="1">
+      <c r="A33" s="41" t="s">
+        <v>60</v>
+      </c>
+      <c r="B33" s="27" t="s">
+        <v>242</v>
+      </c>
+      <c r="C33" s="41"/>
+    </row>
+    <row r="34" spans="1:3" ht="15" customHeight="1">
+      <c r="A34" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="B34" s="27" t="s">
+        <v>243</v>
+      </c>
+      <c r="C34" s="41"/>
+    </row>
+    <row r="35" spans="1:3" ht="15.6">
+      <c r="A35" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="C35" s="20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="15.6">
+      <c r="A36" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="C36" s="20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="15.6">
+      <c r="A37" s="42" t="s">
+        <v>68</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C37" s="20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="B38" s="20" t="s">
+        <v>235</v>
+      </c>
+      <c r="C38" s="20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="42" t="s">
+        <v>72</v>
+      </c>
+      <c r="B39" s="20" t="s">
+        <v>236</v>
+      </c>
+      <c r="C39" s="20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="16" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB570A33-ABD8-4C09-A3B4-18EBA03CD693}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -3608,296 +3976,4 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46ACBD4C-1708-4E7B-88DE-7B19F26CFE31}">
-  <dimension ref="A5:C34"/>
-  <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C27" sqref="A5:C34"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col min="1" max="1" width="21.5546875" customWidth="1"/>
-    <col min="2" max="2" width="70.44140625" customWidth="1"/>
-    <col min="3" max="3" width="45.77734375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="5" spans="1:3">
-      <c r="A5" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="21" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="26" t="s">
-        <v>217</v>
-      </c>
-      <c r="C6" s="22"/>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="26" t="s">
-        <v>218</v>
-      </c>
-      <c r="C7" s="22"/>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="26" t="s">
-        <v>219</v>
-      </c>
-      <c r="C8" s="22"/>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="26" t="s">
-        <v>220</v>
-      </c>
-      <c r="C9" s="22"/>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="26" t="s">
-        <v>221</v>
-      </c>
-      <c r="C10" s="22"/>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="26" t="s">
-        <v>222</v>
-      </c>
-      <c r="C11" s="22"/>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="26" t="s">
-        <v>223</v>
-      </c>
-      <c r="C12" s="22"/>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="26" t="s">
-        <v>224</v>
-      </c>
-      <c r="C13" s="22"/>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="26" t="s">
-        <v>225</v>
-      </c>
-      <c r="C14" s="22"/>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="26" t="s">
-        <v>226</v>
-      </c>
-      <c r="C15" s="22"/>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" s="26" t="s">
-        <v>227</v>
-      </c>
-      <c r="C16" s="22"/>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" s="26" t="s">
-        <v>228</v>
-      </c>
-      <c r="C17" s="22"/>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" s="26" t="s">
-        <v>229</v>
-      </c>
-      <c r="C18" s="22"/>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" s="26" t="s">
-        <v>230</v>
-      </c>
-      <c r="C19" s="22"/>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="B20" s="26" t="s">
-        <v>231</v>
-      </c>
-      <c r="C20" s="22"/>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="B21" s="26" t="s">
-        <v>224</v>
-      </c>
-      <c r="C21" s="22"/>
-    </row>
-    <row r="22" spans="1:3" ht="15.6" customHeight="1">
-      <c r="A22" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="B22" s="26" t="s">
-        <v>223</v>
-      </c>
-      <c r="C22" s="22"/>
-    </row>
-    <row r="23" spans="1:3" ht="13.8" hidden="1" customHeight="1">
-      <c r="A23" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="B23" s="29" t="s">
-        <v>232</v>
-      </c>
-      <c r="C23" s="22"/>
-    </row>
-    <row r="24" spans="1:3" ht="18" hidden="1" customHeight="1">
-      <c r="A24" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="B24" s="29" t="s">
-        <v>233</v>
-      </c>
-      <c r="C24" s="22"/>
-    </row>
-    <row r="25" spans="1:3" hidden="1">
-      <c r="A25" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="B25" s="29" t="s">
-        <v>234</v>
-      </c>
-      <c r="C25" s="22"/>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="B26" s="29" t="s">
-        <v>235</v>
-      </c>
-      <c r="C26" s="22"/>
-    </row>
-    <row r="27" spans="1:3" ht="17.399999999999999" customHeight="1">
-      <c r="A27" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="B27" s="29" t="s">
-        <v>236</v>
-      </c>
-      <c r="C27" s="22"/>
-    </row>
-    <row r="28" spans="1:3" ht="16.8" customHeight="1">
-      <c r="A28" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="B28" s="29" t="s">
-        <v>237</v>
-      </c>
-      <c r="C28" s="22"/>
-    </row>
-    <row r="29" spans="1:3" ht="18" customHeight="1">
-      <c r="A29" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="B29" s="29" t="s">
-        <v>238</v>
-      </c>
-      <c r="C29" s="22"/>
-    </row>
-    <row r="30" spans="1:3" ht="18.600000000000001" customHeight="1">
-      <c r="A30" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="B30" s="29" t="s">
-        <v>239</v>
-      </c>
-      <c r="C30" s="22"/>
-    </row>
-    <row r="31" spans="1:3" ht="15.6" customHeight="1">
-      <c r="A31" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="B31" s="29" t="s">
-        <v>240</v>
-      </c>
-      <c r="C31" s="22"/>
-    </row>
-    <row r="32" spans="1:3" ht="16.8" customHeight="1">
-      <c r="A32" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="B32" s="29" t="s">
-        <v>241</v>
-      </c>
-      <c r="C32" s="22"/>
-    </row>
-    <row r="33" spans="1:3" ht="15.6" customHeight="1">
-      <c r="A33" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="B33" s="29" t="s">
-        <v>242</v>
-      </c>
-      <c r="C33" s="22"/>
-    </row>
-    <row r="34" spans="1:3" ht="15" customHeight="1">
-      <c r="A34" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="B34" s="29" t="s">
-        <v>243</v>
-      </c>
-      <c r="C34" s="22"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
love babar sheet Array Part Added
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AbhishekBiswas\Desktop\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{612CE840-8F80-4B7A-AF2D-372C9D29FCC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F743ACCF-369E-4E2B-BDDA-F31F19E94B7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arrays" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Maths" sheetId="7" r:id="rId5"/>
     <sheet name="Recursion" sheetId="8" r:id="rId6"/>
     <sheet name="Bit magic" sheetId="6" r:id="rId7"/>
+    <sheet name="Love Babbar DSA" sheetId="9" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Matrix!$A$5:$C$29</definedName>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="310">
   <si>
     <t xml:space="preserve">DSA </t>
   </si>
@@ -831,18 +832,154 @@
   </si>
   <si>
     <t>Modular Multiplicative Inverse</t>
+  </si>
+  <si>
+    <t>Reverse the array</t>
+  </si>
+  <si>
+    <t>Find the maximum and minimum element in an array</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Find the "Kth" max and min element of an array </t>
+  </si>
+  <si>
+    <t>Given an array which consists of only 0, 1 and 2. Sort the array without using any sorting algo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Move all the negative elements to one side of the array </t>
+  </si>
+  <si>
+    <t>Find the Union and Intersection of the two sorted arrays.</t>
+  </si>
+  <si>
+    <t>Write a program to cyclically rotate an array by one.</t>
+  </si>
+  <si>
+    <t>find Largest sum contiguous Subarray [V. IMP]</t>
+  </si>
+  <si>
+    <t>Minimise the maximum difference between heights [V.IMP]</t>
+  </si>
+  <si>
+    <t>Minimum no. of Jumps to reach end of an array</t>
+  </si>
+  <si>
+    <t>find duplicate in an array of N+1 Integers</t>
+  </si>
+  <si>
+    <t>Merge 2 sorted arrays without using Extra space.</t>
+  </si>
+  <si>
+    <t>Kadane's Algo [V.V.V.V.V IMP]</t>
+  </si>
+  <si>
+    <t>Merge Intervals</t>
+  </si>
+  <si>
+    <t>Next Permutation</t>
+  </si>
+  <si>
+    <t>Count Inversion</t>
+  </si>
+  <si>
+    <t>Best time to buy and Sell stock</t>
+  </si>
+  <si>
+    <t>find all pairs on integer array whose sum is equal to given number</t>
+  </si>
+  <si>
+    <t>find common elements In 3 sorted arrays</t>
+  </si>
+  <si>
+    <t>Rearrange the array in alternating positive and negative items with O(1) extra space</t>
+  </si>
+  <si>
+    <t>Find if there is any subarray with sum equal to 0</t>
+  </si>
+  <si>
+    <t>Find factorial of a large number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">find maximum product subarray </t>
+  </si>
+  <si>
+    <t>Find longest coinsecutive subsequence</t>
+  </si>
+  <si>
+    <t>Given an array of size n and a number k, fin all elements that appear more than " n/k " times.</t>
+  </si>
+  <si>
+    <t>Maximum profit by buying and selling a share atmost twice</t>
+  </si>
+  <si>
+    <t>Find whether an array is a subset of another array</t>
+  </si>
+  <si>
+    <t>Find the triplet that sum to a given value</t>
+  </si>
+  <si>
+    <t>Trapping Rain water problem</t>
+  </si>
+  <si>
+    <t>Chocolate Distribution problem</t>
+  </si>
+  <si>
+    <t>Smallest Subarray with sum greater than a given value</t>
+  </si>
+  <si>
+    <t>Three way partitioning of an array around a given value</t>
+  </si>
+  <si>
+    <t>Minimum swaps required bring elements less equal K together</t>
+  </si>
+  <si>
+    <t>Minimum no. of operations required to make an array palindrome</t>
+  </si>
+  <si>
+    <t>Median of 2 sorted arrays of equal size</t>
+  </si>
+  <si>
+    <t>Median of 2 sorted arrays of different size</t>
+  </si>
+  <si>
+    <t>Problem Category</t>
+  </si>
+  <si>
+    <t>Problem Statement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Status </t>
+  </si>
+  <si>
+    <t>Arrays Folder</t>
+  </si>
+  <si>
+    <t>Array Folder</t>
+  </si>
+  <si>
+    <t>Sorting Folder</t>
+  </si>
+  <si>
+    <t>Meta (Parent)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1062,79 +1199,92 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2030,7 +2180,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="17" type="noConversion"/>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter>
@@ -2427,7 +2577,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="16" type="noConversion"/>
+  <phoneticPr fontId="17" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3036,7 +3186,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A4:C60" xr:uid="{90C4FD7F-5EC5-490A-B30F-D01CABD8A4B4}"/>
-  <phoneticPr fontId="16" type="noConversion"/>
+  <phoneticPr fontId="17" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3321,7 +3471,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A5:C29" xr:uid="{05A54019-BCB4-4D3D-8A03-2417EABC3558}"/>
-  <phoneticPr fontId="16" type="noConversion"/>
+  <phoneticPr fontId="17" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3442,19 +3592,19 @@
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="44" t="s">
+      <c r="A14" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="45" t="s">
+      <c r="B14" s="43" t="s">
         <v>252</v>
       </c>
-      <c r="C14" s="44"/>
+      <c r="C14" s="42"/>
     </row>
     <row r="15" spans="1:3" ht="15" customHeight="1">
       <c r="A15" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="43" t="s">
+      <c r="B15" s="41" t="s">
         <v>253</v>
       </c>
       <c r="C15" s="28" t="s">
@@ -3539,13 +3689,13 @@
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="44" t="s">
+      <c r="A23" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="B23" s="46" t="s">
+      <c r="B23" s="44" t="s">
         <v>261</v>
       </c>
-      <c r="C23" s="44"/>
+      <c r="C23" s="42"/>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="28" t="s">
@@ -3611,8 +3761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46ACBD4C-1708-4E7B-88DE-7B19F26CFE31}">
   <dimension ref="A5:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3635,332 +3785,335 @@
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="41" t="s">
+      <c r="A6" s="45" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="25" t="s">
         <v>217</v>
       </c>
-      <c r="C6" s="41"/>
+      <c r="C6" s="45"/>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="41" t="s">
+      <c r="A7" s="45" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="25" t="s">
         <v>218</v>
       </c>
-      <c r="C7" s="41"/>
+      <c r="C7" s="45"/>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="41" t="s">
+      <c r="A8" s="45" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="25" t="s">
         <v>219</v>
       </c>
-      <c r="C8" s="41"/>
+      <c r="C8" s="45"/>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="41" t="s">
+      <c r="A9" s="45" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="25" t="s">
         <v>220</v>
       </c>
-      <c r="C9" s="41"/>
+      <c r="C9" s="45"/>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="41" t="s">
+      <c r="A10" s="45" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="25" t="s">
         <v>221</v>
       </c>
-      <c r="C10" s="41"/>
+      <c r="C10" s="45"/>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="41" t="s">
+      <c r="A11" s="45" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="25" t="s">
         <v>222</v>
       </c>
-      <c r="C11" s="41"/>
+      <c r="C11" s="45"/>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="41" t="s">
+      <c r="A12" s="45" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="25" t="s">
         <v>223</v>
       </c>
-      <c r="C12" s="41"/>
+      <c r="C12" s="45"/>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="41" t="s">
+      <c r="A13" s="45" t="s">
         <v>20</v>
       </c>
       <c r="B13" s="25" t="s">
         <v>224</v>
       </c>
-      <c r="C13" s="41"/>
+      <c r="C13" s="45"/>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="41" t="s">
+      <c r="A14" s="45" t="s">
         <v>22</v>
       </c>
       <c r="B14" s="25" t="s">
         <v>225</v>
       </c>
-      <c r="C14" s="41"/>
+      <c r="C14" s="45"/>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="41" t="s">
+      <c r="A15" s="45" t="s">
         <v>24</v>
       </c>
       <c r="B15" s="25" t="s">
         <v>226</v>
       </c>
-      <c r="C15" s="41"/>
+      <c r="C15" s="45"/>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="41" t="s">
+      <c r="A16" s="45" t="s">
         <v>26</v>
       </c>
       <c r="B16" s="25" t="s">
         <v>227</v>
       </c>
-      <c r="C16" s="41"/>
+      <c r="C16" s="45"/>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="41" t="s">
+      <c r="A17" s="45" t="s">
         <v>28</v>
       </c>
       <c r="B17" s="25" t="s">
         <v>228</v>
       </c>
-      <c r="C17" s="41"/>
+      <c r="C17" s="45"/>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="41" t="s">
+      <c r="A18" s="45" t="s">
         <v>30</v>
       </c>
       <c r="B18" s="25" t="s">
         <v>229</v>
       </c>
-      <c r="C18" s="41"/>
+      <c r="C18" s="45"/>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="41" t="s">
+      <c r="A19" s="45" t="s">
         <v>32</v>
       </c>
       <c r="B19" s="25" t="s">
         <v>230</v>
       </c>
-      <c r="C19" s="41"/>
+      <c r="C19" s="45"/>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="42" t="s">
+      <c r="A20" s="28" t="s">
         <v>34</v>
       </c>
       <c r="B20" s="30" t="s">
         <v>231</v>
       </c>
-      <c r="C20" s="42" t="s">
+      <c r="C20" s="28" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="41" t="s">
+      <c r="A21" s="45" t="s">
         <v>36</v>
       </c>
       <c r="B21" s="25" t="s">
         <v>224</v>
       </c>
-      <c r="C21" s="41"/>
+      <c r="C21" s="45"/>
     </row>
     <row r="22" spans="1:3" ht="15.6" customHeight="1">
-      <c r="A22" s="41" t="s">
+      <c r="A22" s="45" t="s">
         <v>38</v>
       </c>
       <c r="B22" s="25" t="s">
         <v>223</v>
       </c>
-      <c r="C22" s="41"/>
+      <c r="C22" s="45"/>
     </row>
     <row r="23" spans="1:3" ht="13.8" hidden="1" customHeight="1">
-      <c r="A23" s="41" t="s">
+      <c r="A23" s="45" t="s">
         <v>40</v>
       </c>
       <c r="B23" s="27" t="s">
         <v>232</v>
       </c>
-      <c r="C23" s="41"/>
+      <c r="C23" s="45"/>
     </row>
     <row r="24" spans="1:3" ht="18" hidden="1" customHeight="1">
-      <c r="A24" s="41" t="s">
+      <c r="A24" s="45" t="s">
         <v>42</v>
       </c>
       <c r="B24" s="27" t="s">
         <v>233</v>
       </c>
-      <c r="C24" s="41"/>
+      <c r="C24" s="45"/>
     </row>
     <row r="25" spans="1:3" hidden="1">
-      <c r="A25" s="41" t="s">
+      <c r="A25" s="45" t="s">
         <v>44</v>
       </c>
       <c r="B25" s="27" t="s">
         <v>234</v>
       </c>
-      <c r="C25" s="41"/>
+      <c r="C25" s="45"/>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="42" t="s">
+      <c r="A26" s="28" t="s">
         <v>46</v>
       </c>
       <c r="B26" s="29" t="s">
         <v>235</v>
       </c>
-      <c r="C26" s="42" t="s">
+      <c r="C26" s="28" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="17.399999999999999" customHeight="1">
-      <c r="A27" s="42" t="s">
+      <c r="A27" s="28" t="s">
         <v>48</v>
       </c>
       <c r="B27" s="29" t="s">
         <v>236</v>
       </c>
-      <c r="C27" s="42" t="s">
+      <c r="C27" s="28" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="16.8" customHeight="1">
-      <c r="A28" s="42" t="s">
+      <c r="A28" s="28" t="s">
         <v>50</v>
       </c>
       <c r="B28" s="29" t="s">
         <v>237</v>
       </c>
-      <c r="C28" s="42" t="s">
+      <c r="C28" s="28" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="18" customHeight="1">
-      <c r="A29" s="41" t="s">
+      <c r="A29" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="B29" s="27" t="s">
+      <c r="B29" s="29" t="s">
         <v>238</v>
       </c>
-      <c r="C29" s="41"/>
+      <c r="C29" s="28" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="30" spans="1:3" ht="18.600000000000001" customHeight="1">
-      <c r="A30" s="41" t="s">
+      <c r="A30" s="45" t="s">
         <v>54</v>
       </c>
       <c r="B30" s="27" t="s">
         <v>239</v>
       </c>
-      <c r="C30" s="41"/>
+      <c r="C30" s="45"/>
     </row>
     <row r="31" spans="1:3" ht="15.6" customHeight="1">
-      <c r="A31" s="41" t="s">
+      <c r="A31" s="45" t="s">
         <v>56</v>
       </c>
       <c r="B31" s="27" t="s">
         <v>240</v>
       </c>
-      <c r="C31" s="41"/>
+      <c r="C31" s="45"/>
     </row>
     <row r="32" spans="1:3" ht="16.8" customHeight="1">
-      <c r="A32" s="41" t="s">
+      <c r="A32" s="45" t="s">
         <v>58</v>
       </c>
       <c r="B32" s="27" t="s">
         <v>241</v>
       </c>
-      <c r="C32" s="41"/>
+      <c r="C32" s="45"/>
     </row>
     <row r="33" spans="1:3" ht="15.6" customHeight="1">
-      <c r="A33" s="41" t="s">
+      <c r="A33" s="45" t="s">
         <v>60</v>
       </c>
       <c r="B33" s="27" t="s">
         <v>242</v>
       </c>
-      <c r="C33" s="41"/>
+      <c r="C33" s="45"/>
     </row>
     <row r="34" spans="1:3" ht="15" customHeight="1">
-      <c r="A34" s="41" t="s">
+      <c r="A34" s="45" t="s">
         <v>62</v>
       </c>
       <c r="B34" s="27" t="s">
         <v>243</v>
       </c>
-      <c r="C34" s="41"/>
+      <c r="C34" s="45"/>
     </row>
     <row r="35" spans="1:3" ht="15.6">
-      <c r="A35" s="42" t="s">
+      <c r="A35" s="28" t="s">
         <v>64</v>
       </c>
       <c r="B35" s="9" t="s">
         <v>233</v>
       </c>
-      <c r="C35" s="20" t="s">
+      <c r="C35" s="46" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="15.6">
-      <c r="A36" s="42" t="s">
+      <c r="A36" s="28" t="s">
         <v>66</v>
       </c>
       <c r="B36" s="9" t="s">
         <v>232</v>
       </c>
-      <c r="C36" s="20" t="s">
+      <c r="C36" s="46" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="15.6">
-      <c r="A37" s="42" t="s">
+      <c r="A37" s="28" t="s">
         <v>68</v>
       </c>
       <c r="B37" s="9" t="s">
         <v>234</v>
       </c>
-      <c r="C37" s="20" t="s">
+      <c r="C37" s="46" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38" s="42" t="s">
+      <c r="A38" s="28" t="s">
         <v>70</v>
       </c>
       <c r="B38" s="20" t="s">
         <v>235</v>
       </c>
-      <c r="C38" s="20" t="s">
+      <c r="C38" s="46" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="39" spans="1:3">
-      <c r="A39" s="42" t="s">
+      <c r="A39" s="28" t="s">
         <v>72</v>
       </c>
       <c r="B39" s="20" t="s">
         <v>236</v>
       </c>
-      <c r="C39" s="20" t="s">
+      <c r="C39" s="46" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="16" type="noConversion"/>
+  <phoneticPr fontId="17" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3976,4 +4129,526 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AE24439-416F-43FF-9A18-3B2A875B7F08}">
+  <dimension ref="A1:E39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="25.5546875" customWidth="1"/>
+    <col min="2" max="2" width="29.5546875" customWidth="1"/>
+    <col min="3" max="3" width="105" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="E1" s="40"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="50" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>267</v>
+      </c>
+      <c r="D4" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="50" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="50" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>268</v>
+      </c>
+      <c r="D5" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="50" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>269</v>
+      </c>
+      <c r="D6" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="50" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="47" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="49" t="s">
+        <v>270</v>
+      </c>
+      <c r="D7" s="48"/>
+      <c r="E7" s="48"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="47" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="49" t="s">
+        <v>271</v>
+      </c>
+      <c r="D8" s="48"/>
+      <c r="E8" s="48"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="47" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="49" t="s">
+        <v>272</v>
+      </c>
+      <c r="D9" s="48"/>
+      <c r="E9" s="48"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="47" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="49" t="s">
+        <v>273</v>
+      </c>
+      <c r="D10" s="48"/>
+      <c r="E10" s="48"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="47" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="49" t="s">
+        <v>274</v>
+      </c>
+      <c r="D11" s="48"/>
+      <c r="E11" s="48"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="49" t="s">
+        <v>275</v>
+      </c>
+      <c r="D12" s="48"/>
+      <c r="E12" s="48"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="49" t="s">
+        <v>276</v>
+      </c>
+      <c r="D13" s="48"/>
+      <c r="E13" s="48"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="49" t="s">
+        <v>277</v>
+      </c>
+      <c r="D14" s="48"/>
+      <c r="E14" s="48"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="47" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="49" t="s">
+        <v>278</v>
+      </c>
+      <c r="D15" s="48"/>
+      <c r="E15" s="48"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="47" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="49" t="s">
+        <v>279</v>
+      </c>
+      <c r="D16" s="48"/>
+      <c r="E16" s="48"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="47" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="49" t="s">
+        <v>280</v>
+      </c>
+      <c r="D17" s="48"/>
+      <c r="E17" s="48"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="49" t="s">
+        <v>281</v>
+      </c>
+      <c r="D18" s="48"/>
+      <c r="E18" s="48"/>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="47" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="49" t="s">
+        <v>282</v>
+      </c>
+      <c r="D19" s="48"/>
+      <c r="E19" s="48"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="49" t="s">
+        <v>283</v>
+      </c>
+      <c r="D20" s="48"/>
+      <c r="E20" s="48"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="49" t="s">
+        <v>284</v>
+      </c>
+      <c r="D21" s="48"/>
+      <c r="E21" s="48"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="49" t="s">
+        <v>285</v>
+      </c>
+      <c r="D22" s="48"/>
+      <c r="E22" s="48"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="47" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="49" t="s">
+        <v>286</v>
+      </c>
+      <c r="D23" s="48"/>
+      <c r="E23" s="48"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" s="49" t="s">
+        <v>287</v>
+      </c>
+      <c r="D24" s="48"/>
+      <c r="E24" s="48"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="47" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" s="49" t="s">
+        <v>288</v>
+      </c>
+      <c r="D25" s="48"/>
+      <c r="E25" s="48"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="47" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="49" t="s">
+        <v>289</v>
+      </c>
+      <c r="D26" s="48"/>
+      <c r="E26" s="48"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="47" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="49" t="s">
+        <v>290</v>
+      </c>
+      <c r="D27" s="48"/>
+      <c r="E27" s="48"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="47" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="49" t="s">
+        <v>291</v>
+      </c>
+      <c r="D28" s="48"/>
+      <c r="E28" s="48"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="47" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" s="49" t="s">
+        <v>292</v>
+      </c>
+      <c r="D29" s="48"/>
+      <c r="E29" s="48"/>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="47" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" s="49" t="s">
+        <v>293</v>
+      </c>
+      <c r="D30" s="48"/>
+      <c r="E30" s="48"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="47" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" s="49" t="s">
+        <v>294</v>
+      </c>
+      <c r="D31" s="48"/>
+      <c r="E31" s="48"/>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="47" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" s="49" t="s">
+        <v>295</v>
+      </c>
+      <c r="D32" s="48"/>
+      <c r="E32" s="48"/>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="47" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" s="49" t="s">
+        <v>296</v>
+      </c>
+      <c r="D33" s="48"/>
+      <c r="E33" s="48"/>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="47" t="s">
+        <v>66</v>
+      </c>
+      <c r="B34" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34" s="49" t="s">
+        <v>297</v>
+      </c>
+      <c r="D34" s="48"/>
+      <c r="E34" s="48"/>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="47" t="s">
+        <v>68</v>
+      </c>
+      <c r="B35" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35" s="49" t="s">
+        <v>298</v>
+      </c>
+      <c r="D35" s="48"/>
+      <c r="E35" s="48"/>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="47" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C36" s="49" t="s">
+        <v>299</v>
+      </c>
+      <c r="D36" s="48"/>
+      <c r="E36" s="48"/>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="47" t="s">
+        <v>72</v>
+      </c>
+      <c r="B37" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C37" s="49" t="s">
+        <v>300</v>
+      </c>
+      <c r="D37" s="48"/>
+      <c r="E37" s="48"/>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="47" t="s">
+        <v>74</v>
+      </c>
+      <c r="B38" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38" s="49" t="s">
+        <v>301</v>
+      </c>
+      <c r="D38" s="48"/>
+      <c r="E38" s="48"/>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="47" t="s">
+        <v>76</v>
+      </c>
+      <c r="B39" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C39" s="49" t="s">
+        <v>302</v>
+      </c>
+      <c r="D39" s="48"/>
+      <c r="E39" s="48"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="17" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
string and hashing added
sorry for late commit and push
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AbhishekBiswas\Desktop\DSA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhishekbiswas/Desktop/DSA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7721CB6-816D-4D43-A852-9B11B3D6C67E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36917FC4-52FE-5842-8EA6-5580FBCCE11E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" firstSheet="2" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arrays" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="Bit magic" sheetId="6" r:id="rId8"/>
     <sheet name="Bind75" sheetId="11" r:id="rId9"/>
     <sheet name="Love Babbar DSA" sheetId="9" r:id="rId10"/>
+    <sheet name="Strings" sheetId="12" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Matrix!$A$2:$C$26</definedName>
@@ -1255,7 +1256,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="26">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1894,16 +1895,16 @@
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.5546875" style="45" customWidth="1"/>
-    <col min="2" max="2" width="53.5546875" style="45" customWidth="1"/>
+    <col min="1" max="1" width="23.5" style="45" customWidth="1"/>
+    <col min="2" max="2" width="53.5" style="45" customWidth="1"/>
     <col min="3" max="3" width="9" style="45"/>
-    <col min="4" max="4" width="18.109375" style="45" customWidth="1"/>
+    <col min="4" max="4" width="18.1640625" style="45" customWidth="1"/>
     <col min="5" max="16384" width="9" style="45"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1914,7 +1915,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="51" t="s">
         <v>4</v>
       </c>
@@ -1925,7 +1926,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="51" t="s">
         <v>7</v>
       </c>
@@ -1936,7 +1937,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="51" t="s">
         <v>9</v>
       </c>
@@ -1947,7 +1948,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="51" t="s">
         <v>11</v>
       </c>
@@ -1958,7 +1959,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="51" t="s">
         <v>13</v>
       </c>
@@ -1969,7 +1970,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="51" t="s">
         <v>15</v>
       </c>
@@ -1980,7 +1981,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="51" t="s">
         <v>17</v>
       </c>
@@ -1991,7 +1992,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="51" t="s">
         <v>19</v>
       </c>
@@ -2002,7 +2003,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="51" t="s">
         <v>21</v>
       </c>
@@ -2013,7 +2014,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="51" t="s">
         <v>23</v>
       </c>
@@ -2024,7 +2025,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="51" t="s">
         <v>25</v>
       </c>
@@ -2035,7 +2036,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="53" t="s">
         <v>27</v>
       </c>
@@ -2044,7 +2045,7 @@
       </c>
       <c r="C13" s="53"/>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="53" t="s">
         <v>29</v>
       </c>
@@ -2053,7 +2054,7 @@
       </c>
       <c r="C14" s="53"/>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="51" t="s">
         <v>31</v>
       </c>
@@ -2064,7 +2065,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="51" t="s">
         <v>33</v>
       </c>
@@ -2075,7 +2076,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="51" t="s">
         <v>35</v>
       </c>
@@ -2086,7 +2087,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="51" t="s">
         <v>37</v>
       </c>
@@ -2097,7 +2098,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="51" t="s">
         <v>39</v>
       </c>
@@ -2108,7 +2109,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="51" t="s">
         <v>41</v>
       </c>
@@ -2119,7 +2120,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="53" t="s">
         <v>43</v>
       </c>
@@ -2128,7 +2129,7 @@
       </c>
       <c r="C21" s="53"/>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="51" t="s">
         <v>45</v>
       </c>
@@ -2139,7 +2140,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="51" t="s">
         <v>47</v>
       </c>
@@ -2150,7 +2151,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="51" t="s">
         <v>49</v>
       </c>
@@ -2161,7 +2162,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="51" t="s">
         <v>51</v>
       </c>
@@ -2172,7 +2173,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="51" t="s">
         <v>53</v>
       </c>
@@ -2183,7 +2184,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="51" t="s">
         <v>55</v>
       </c>
@@ -2194,7 +2195,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="51" t="s">
         <v>57</v>
       </c>
@@ -2205,7 +2206,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="51" t="s">
         <v>59</v>
       </c>
@@ -2216,7 +2217,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="51" t="s">
         <v>61</v>
       </c>
@@ -2227,7 +2228,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="51" t="s">
         <v>63</v>
       </c>
@@ -2238,7 +2239,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="51" t="s">
         <v>65</v>
       </c>
@@ -2249,7 +2250,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="53" t="s">
         <v>67</v>
       </c>
@@ -2258,7 +2259,7 @@
       </c>
       <c r="C33" s="53"/>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="51" t="s">
         <v>69</v>
       </c>
@@ -2269,7 +2270,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="51" t="s">
         <v>71</v>
       </c>
@@ -2280,7 +2281,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="51" t="s">
         <v>73</v>
       </c>
@@ -2291,7 +2292,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="51" t="s">
         <v>75</v>
       </c>
@@ -2302,7 +2303,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="51" t="s">
         <v>77</v>
       </c>
@@ -2313,7 +2314,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="51" t="s">
         <v>79</v>
       </c>
@@ -2324,7 +2325,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="51" t="s">
         <v>81</v>
       </c>
@@ -2335,7 +2336,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="51" t="s">
         <v>83</v>
       </c>
@@ -2346,7 +2347,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="51" t="s">
         <v>85</v>
       </c>
@@ -2357,7 +2358,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="51" t="s">
         <v>87</v>
       </c>
@@ -2368,7 +2369,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="51" t="s">
         <v>88</v>
       </c>
@@ -2379,7 +2380,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="51" t="s">
         <v>89</v>
       </c>
@@ -2390,7 +2391,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="53" t="s">
         <v>90</v>
       </c>
@@ -2399,7 +2400,7 @@
       </c>
       <c r="C46" s="53"/>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="51" t="s">
         <v>92</v>
       </c>
@@ -2410,7 +2411,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="51" t="s">
         <v>94</v>
       </c>
@@ -2421,7 +2422,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="51" t="s">
         <v>95</v>
       </c>
@@ -2432,7 +2433,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="51" t="s">
         <v>97</v>
       </c>
@@ -2443,7 +2444,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="51" t="s">
         <v>99</v>
       </c>
@@ -2454,7 +2455,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="51" t="s">
         <v>101</v>
       </c>
@@ -2465,7 +2466,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="51" t="s">
         <v>103</v>
       </c>
@@ -2476,7 +2477,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="51" t="s">
         <v>105</v>
       </c>
@@ -2487,7 +2488,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="51" t="s">
         <v>107</v>
       </c>
@@ -2516,15 +2517,15 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.5546875" customWidth="1"/>
-    <col min="2" max="2" width="29.5546875" customWidth="1"/>
+    <col min="1" max="1" width="25.5" customWidth="1"/>
+    <col min="2" max="2" width="29.5" customWidth="1"/>
     <col min="3" max="3" width="105" customWidth="1"/>
     <col min="5" max="5" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -2541,7 +2542,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="42" t="s">
         <v>4</v>
       </c>
@@ -2558,7 +2559,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="42" t="s">
         <v>7</v>
       </c>
@@ -2575,7 +2576,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="42" t="s">
         <v>9</v>
       </c>
@@ -2592,7 +2593,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="42" t="s">
         <v>11</v>
       </c>
@@ -2609,7 +2610,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="42" t="s">
         <v>13</v>
       </c>
@@ -2626,7 +2627,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="42" t="s">
         <v>15</v>
       </c>
@@ -2643,7 +2644,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="42" t="s">
         <v>17</v>
       </c>
@@ -2660,7 +2661,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="42" t="s">
         <v>19</v>
       </c>
@@ -2677,7 +2678,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="39" t="s">
         <v>21</v>
       </c>
@@ -2690,7 +2691,7 @@
       <c r="D10" s="40"/>
       <c r="E10" s="40"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="39" t="s">
         <v>23</v>
       </c>
@@ -2703,7 +2704,7 @@
       <c r="D11" s="40"/>
       <c r="E11" s="40"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="39" t="s">
         <v>25</v>
       </c>
@@ -2716,7 +2717,7 @@
       <c r="D12" s="40"/>
       <c r="E12" s="40"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="39" t="s">
         <v>27</v>
       </c>
@@ -2729,7 +2730,7 @@
       <c r="D13" s="40"/>
       <c r="E13" s="40"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="39" t="s">
         <v>29</v>
       </c>
@@ -2742,7 +2743,7 @@
       <c r="D14" s="40"/>
       <c r="E14" s="40"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="39" t="s">
         <v>31</v>
       </c>
@@ -2755,7 +2756,7 @@
       <c r="D15" s="40"/>
       <c r="E15" s="40"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="39" t="s">
         <v>33</v>
       </c>
@@ -2768,7 +2769,7 @@
       <c r="D16" s="40"/>
       <c r="E16" s="40"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="39" t="s">
         <v>35</v>
       </c>
@@ -2781,7 +2782,7 @@
       <c r="D17" s="40"/>
       <c r="E17" s="40"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="39" t="s">
         <v>37</v>
       </c>
@@ -2794,7 +2795,7 @@
       <c r="D18" s="40"/>
       <c r="E18" s="40"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="39" t="s">
         <v>39</v>
       </c>
@@ -2807,7 +2808,7 @@
       <c r="D19" s="40"/>
       <c r="E19" s="40"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="39" t="s">
         <v>41</v>
       </c>
@@ -2820,7 +2821,7 @@
       <c r="D20" s="40"/>
       <c r="E20" s="40"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="39" t="s">
         <v>43</v>
       </c>
@@ -2833,7 +2834,7 @@
       <c r="D21" s="40"/>
       <c r="E21" s="40"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="39" t="s">
         <v>45</v>
       </c>
@@ -2846,7 +2847,7 @@
       <c r="D22" s="40"/>
       <c r="E22" s="40"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="39" t="s">
         <v>47</v>
       </c>
@@ -2859,7 +2860,7 @@
       <c r="D23" s="40"/>
       <c r="E23" s="40"/>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="39" t="s">
         <v>49</v>
       </c>
@@ -2872,7 +2873,7 @@
       <c r="D24" s="40"/>
       <c r="E24" s="40"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="39" t="s">
         <v>51</v>
       </c>
@@ -2885,7 +2886,7 @@
       <c r="D25" s="40"/>
       <c r="E25" s="40"/>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="39" t="s">
         <v>53</v>
       </c>
@@ -2898,7 +2899,7 @@
       <c r="D26" s="40"/>
       <c r="E26" s="40"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="39" t="s">
         <v>55</v>
       </c>
@@ -2911,7 +2912,7 @@
       <c r="D27" s="40"/>
       <c r="E27" s="40"/>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="39" t="s">
         <v>57</v>
       </c>
@@ -2924,7 +2925,7 @@
       <c r="D28" s="40"/>
       <c r="E28" s="40"/>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="39" t="s">
         <v>59</v>
       </c>
@@ -2937,7 +2938,7 @@
       <c r="D29" s="40"/>
       <c r="E29" s="40"/>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="39" t="s">
         <v>61</v>
       </c>
@@ -2950,7 +2951,7 @@
       <c r="D30" s="40"/>
       <c r="E30" s="40"/>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="39" t="s">
         <v>63</v>
       </c>
@@ -2963,7 +2964,7 @@
       <c r="D31" s="40"/>
       <c r="E31" s="40"/>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="39" t="s">
         <v>65</v>
       </c>
@@ -2976,7 +2977,7 @@
       <c r="D32" s="40"/>
       <c r="E32" s="40"/>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="39" t="s">
         <v>67</v>
       </c>
@@ -2989,7 +2990,7 @@
       <c r="D33" s="40"/>
       <c r="E33" s="40"/>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="39" t="s">
         <v>69</v>
       </c>
@@ -3002,7 +3003,7 @@
       <c r="D34" s="40"/>
       <c r="E34" s="40"/>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="39" t="s">
         <v>71</v>
       </c>
@@ -3015,7 +3016,7 @@
       <c r="D35" s="40"/>
       <c r="E35" s="40"/>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="39" t="s">
         <v>73</v>
       </c>
@@ -3028,7 +3029,7 @@
       <c r="D36" s="40"/>
       <c r="E36" s="40"/>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="39" t="s">
         <v>75</v>
       </c>
@@ -3043,6 +3044,18 @@
     </row>
   </sheetData>
   <phoneticPr fontId="16" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F6774DA-A619-B247-A86A-A8FA24358593}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3055,14 +3068,14 @@
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.5546875" customWidth="1"/>
+    <col min="1" max="1" width="19.5" customWidth="1"/>
     <col min="2" max="2" width="43.6640625" customWidth="1"/>
-    <col min="3" max="3" width="20.77734375" customWidth="1"/>
+    <col min="3" max="3" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -3073,7 +3086,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.6">
+    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -3084,7 +3097,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.6">
+    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -3095,7 +3108,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.6">
+    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -3106,7 +3119,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.6">
+    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -3117,7 +3130,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.6">
+    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -3128,7 +3141,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.6">
+    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
@@ -3139,7 +3152,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.6">
+    <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>17</v>
       </c>
@@ -3150,7 +3163,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.6">
+    <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>19</v>
       </c>
@@ -3161,7 +3174,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.6">
+    <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>21</v>
       </c>
@@ -3172,7 +3185,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.6">
+    <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>23</v>
       </c>
@@ -3183,7 +3196,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.6">
+    <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>25</v>
       </c>
@@ -3194,7 +3207,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.6">
+    <row r="13" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>27</v>
       </c>
@@ -3205,7 +3218,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15.6">
+    <row r="14" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="25" t="s">
         <v>29</v>
       </c>
@@ -3214,7 +3227,7 @@
       </c>
       <c r="C14" s="27"/>
     </row>
-    <row r="15" spans="1:3" ht="15.6">
+    <row r="15" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="25" t="s">
         <v>31</v>
       </c>
@@ -3223,7 +3236,7 @@
       </c>
       <c r="C15" s="27"/>
     </row>
-    <row r="16" spans="1:3" ht="15.6">
+    <row r="16" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="25" t="s">
         <v>33</v>
       </c>
@@ -3232,7 +3245,7 @@
       </c>
       <c r="C16" s="27"/>
     </row>
-    <row r="17" spans="1:3" ht="15.6">
+    <row r="17" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="25" t="s">
         <v>35</v>
       </c>
@@ -3241,7 +3254,7 @@
       </c>
       <c r="C17" s="27"/>
     </row>
-    <row r="18" spans="1:3" ht="15.6">
+    <row r="18" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="25" t="s">
         <v>37</v>
       </c>
@@ -3250,7 +3263,7 @@
       </c>
       <c r="C18" s="27"/>
     </row>
-    <row r="19" spans="1:3" ht="15.6">
+    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>39</v>
       </c>
@@ -3261,7 +3274,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.6">
+    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>41</v>
       </c>
@@ -3272,7 +3285,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15.6">
+    <row r="21" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>43</v>
       </c>
@@ -3283,7 +3296,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15.6">
+    <row r="22" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="25" t="s">
         <v>45</v>
       </c>
@@ -3292,7 +3305,7 @@
       </c>
       <c r="C22" s="27"/>
     </row>
-    <row r="23" spans="1:3" ht="15.6">
+    <row r="23" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="25" t="s">
         <v>47</v>
       </c>
@@ -3301,7 +3314,7 @@
       </c>
       <c r="C23" s="27"/>
     </row>
-    <row r="24" spans="1:3" ht="15.6">
+    <row r="24" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>49</v>
       </c>
@@ -3312,7 +3325,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15.6">
+    <row r="25" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>51</v>
       </c>
@@ -3323,7 +3336,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15.6">
+    <row r="26" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="25" t="s">
         <v>53</v>
       </c>
@@ -3332,7 +3345,7 @@
       </c>
       <c r="C26" s="27"/>
     </row>
-    <row r="27" spans="1:3" ht="15.6">
+    <row r="27" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="25" t="s">
         <v>55</v>
       </c>
@@ -3341,7 +3354,7 @@
       </c>
       <c r="C27" s="27"/>
     </row>
-    <row r="28" spans="1:3" ht="15.6">
+    <row r="28" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>57</v>
       </c>
@@ -3352,7 +3365,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15.6">
+    <row r="29" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>59</v>
       </c>
@@ -3363,7 +3376,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.6">
+    <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="25" t="s">
         <v>61</v>
       </c>
@@ -3372,7 +3385,7 @@
       </c>
       <c r="C30" s="27"/>
     </row>
-    <row r="31" spans="1:3" ht="15.6">
+    <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>63</v>
       </c>
@@ -3383,7 +3396,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15.6">
+    <row r="32" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="25" t="s">
         <v>65</v>
       </c>
@@ -3392,7 +3405,7 @@
       </c>
       <c r="C32" s="27"/>
     </row>
-    <row r="33" spans="1:3" ht="15.6">
+    <row r="33" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>67</v>
       </c>
@@ -3403,7 +3416,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="15.6">
+    <row r="34" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="25" t="s">
         <v>69</v>
       </c>
@@ -3412,7 +3425,7 @@
       </c>
       <c r="C34" s="27"/>
     </row>
-    <row r="35" spans="1:3" ht="15.6">
+    <row r="35" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>71</v>
       </c>
@@ -3423,7 +3436,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="15.6">
+    <row r="36" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>73</v>
       </c>
@@ -3448,15 +3461,15 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.44140625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="19.5" style="5" customWidth="1"/>
     <col min="2" max="2" width="58.6640625" style="5" customWidth="1"/>
     <col min="3" max="3" width="20.6640625" style="5" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="5"/>
+    <col min="4" max="16384" width="8.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -3467,7 +3480,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.6">
+    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
@@ -3478,7 +3491,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.6">
+    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
@@ -3489,7 +3502,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.6">
+    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>9</v>
       </c>
@@ -3500,7 +3513,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.6">
+    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>11</v>
       </c>
@@ -3511,7 +3524,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.6">
+    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>13</v>
       </c>
@@ -3522,7 +3535,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.6">
+    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>15</v>
       </c>
@@ -3533,7 +3546,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.6">
+    <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>17</v>
       </c>
@@ -3544,7 +3557,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.6">
+    <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>19</v>
       </c>
@@ -3555,7 +3568,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.6">
+    <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>21</v>
       </c>
@@ -3566,7 +3579,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.6">
+    <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>23</v>
       </c>
@@ -3577,7 +3590,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.6">
+    <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>25</v>
       </c>
@@ -3588,7 +3601,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.6">
+    <row r="13" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>27</v>
       </c>
@@ -3599,7 +3612,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15.6">
+    <row r="14" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>29</v>
       </c>
@@ -3610,7 +3623,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15.6">
+    <row r="15" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>31</v>
       </c>
@@ -3621,7 +3634,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.6">
+    <row r="16" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>33</v>
       </c>
@@ -3632,7 +3645,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.6">
+    <row r="17" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>35</v>
       </c>
@@ -3643,7 +3656,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.6">
+    <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>37</v>
       </c>
@@ -3654,7 +3667,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15.6">
+    <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="30" t="s">
         <v>39</v>
       </c>
@@ -3666,7 +3679,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15.6">
+    <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="30" t="s">
         <v>41</v>
       </c>
@@ -3675,7 +3688,7 @@
       </c>
       <c r="C20" s="30"/>
     </row>
-    <row r="21" spans="1:5" ht="15.6">
+    <row r="21" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="30" t="s">
         <v>43</v>
       </c>
@@ -3684,7 +3697,7 @@
       </c>
       <c r="C21" s="30"/>
     </row>
-    <row r="22" spans="1:5" ht="15.6">
+    <row r="22" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
         <v>45</v>
       </c>
@@ -3695,7 +3708,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15.6">
+    <row r="23" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
         <v>47</v>
       </c>
@@ -3706,7 +3719,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15.6">
+    <row r="24" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
         <v>49</v>
       </c>
@@ -3717,7 +3730,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15.6">
+    <row r="25" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="30" t="s">
         <v>51</v>
       </c>
@@ -3726,7 +3739,7 @@
       </c>
       <c r="C25" s="30"/>
     </row>
-    <row r="26" spans="1:5" ht="15.6">
+    <row r="26" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>53</v>
       </c>
@@ -3737,7 +3750,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15.6">
+    <row r="27" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
         <v>55</v>
       </c>
@@ -3748,7 +3761,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15.6">
+    <row r="28" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="30" t="s">
         <v>57</v>
       </c>
@@ -3757,7 +3770,7 @@
       </c>
       <c r="C28" s="30"/>
     </row>
-    <row r="29" spans="1:5" ht="15.6">
+    <row r="29" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="30" t="s">
         <v>59</v>
       </c>
@@ -3766,7 +3779,7 @@
       </c>
       <c r="C29" s="30"/>
     </row>
-    <row r="30" spans="1:5" ht="15.6">
+    <row r="30" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="30" t="s">
         <v>61</v>
       </c>
@@ -3775,7 +3788,7 @@
       </c>
       <c r="C30" s="30"/>
     </row>
-    <row r="31" spans="1:5" ht="15.6">
+    <row r="31" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="30" t="s">
         <v>63</v>
       </c>
@@ -3784,7 +3797,7 @@
       </c>
       <c r="C31" s="30"/>
     </row>
-    <row r="32" spans="1:5" ht="15.6">
+    <row r="32" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="30" t="s">
         <v>65</v>
       </c>
@@ -3793,7 +3806,7 @@
       </c>
       <c r="C32" s="30"/>
     </row>
-    <row r="33" spans="1:3" ht="15.6">
+    <row r="33" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="30" t="s">
         <v>67</v>
       </c>
@@ -3802,7 +3815,7 @@
       </c>
       <c r="C33" s="30"/>
     </row>
-    <row r="34" spans="1:3" ht="15.6">
+    <row r="34" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="30" t="s">
         <v>69</v>
       </c>
@@ -3811,7 +3824,7 @@
       </c>
       <c r="C34" s="30"/>
     </row>
-    <row r="35" spans="1:3" ht="15.6">
+    <row r="35" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
         <v>71</v>
       </c>
@@ -3822,7 +3835,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="15.6">
+    <row r="36" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
         <v>73</v>
       </c>
@@ -3833,7 +3846,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15.6">
+    <row r="37" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="30" t="s">
         <v>75</v>
       </c>
@@ -3842,7 +3855,7 @@
       </c>
       <c r="C37" s="30"/>
     </row>
-    <row r="38" spans="1:3" ht="15.6">
+    <row r="38" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="30" t="s">
         <v>77</v>
       </c>
@@ -3851,7 +3864,7 @@
       </c>
       <c r="C38" s="30"/>
     </row>
-    <row r="39" spans="1:3" ht="15.6">
+    <row r="39" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="30" t="s">
         <v>79</v>
       </c>
@@ -3860,7 +3873,7 @@
       </c>
       <c r="C39" s="30"/>
     </row>
-    <row r="40" spans="1:3" ht="15.6">
+    <row r="40" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="30" t="s">
         <v>81</v>
       </c>
@@ -3869,7 +3882,7 @@
       </c>
       <c r="C40" s="30"/>
     </row>
-    <row r="41" spans="1:3" ht="15.6">
+    <row r="41" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
         <v>83</v>
       </c>
@@ -3880,7 +3893,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="15.6">
+    <row r="42" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="30" t="s">
         <v>85</v>
       </c>
@@ -3889,7 +3902,7 @@
       </c>
       <c r="C42" s="30"/>
     </row>
-    <row r="43" spans="1:3" ht="15.6">
+    <row r="43" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="30" t="s">
         <v>87</v>
       </c>
@@ -3898,7 +3911,7 @@
       </c>
       <c r="C43" s="30"/>
     </row>
-    <row r="44" spans="1:3" ht="15.6">
+    <row r="44" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="30" t="s">
         <v>88</v>
       </c>
@@ -3907,7 +3920,7 @@
       </c>
       <c r="C44" s="30"/>
     </row>
-    <row r="45" spans="1:3" ht="15.6">
+    <row r="45" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="30" t="s">
         <v>89</v>
       </c>
@@ -3916,7 +3929,7 @@
       </c>
       <c r="C45" s="30"/>
     </row>
-    <row r="46" spans="1:3" ht="15.6">
+    <row r="46" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
         <v>90</v>
       </c>
@@ -3927,7 +3940,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="15.6">
+    <row r="47" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
         <v>92</v>
       </c>
@@ -3938,7 +3951,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="15.6">
+    <row r="48" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="30" t="s">
         <v>94</v>
       </c>
@@ -3947,7 +3960,7 @@
       </c>
       <c r="C48" s="30"/>
     </row>
-    <row r="49" spans="1:3" ht="15.6">
+    <row r="49" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
         <v>95</v>
       </c>
@@ -3958,7 +3971,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="15.6">
+    <row r="50" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="30" t="s">
         <v>97</v>
       </c>
@@ -3967,7 +3980,7 @@
       </c>
       <c r="C50" s="30"/>
     </row>
-    <row r="51" spans="1:3" ht="15.6">
+    <row r="51" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
         <v>99</v>
       </c>
@@ -3978,7 +3991,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="15.6">
+    <row r="52" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
         <v>101</v>
       </c>
@@ -3989,7 +4002,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="15.6">
+    <row r="53" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
         <v>103</v>
       </c>
@@ -4000,7 +4013,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="15.6">
+    <row r="54" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
         <v>105</v>
       </c>
@@ -4011,7 +4024,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="15.6">
+    <row r="55" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
         <v>107</v>
       </c>
@@ -4022,7 +4035,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="15.6">
+    <row r="56" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="30" t="s">
         <v>191</v>
       </c>
@@ -4031,7 +4044,7 @@
       </c>
       <c r="C56" s="30"/>
     </row>
-    <row r="57" spans="1:3" ht="15.6">
+    <row r="57" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="6" t="s">
         <v>192</v>
       </c>
@@ -4057,14 +4070,14 @@
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.5546875" customWidth="1"/>
-    <col min="2" max="2" width="56.44140625" customWidth="1"/>
-    <col min="3" max="3" width="26.88671875" customWidth="1"/>
+    <col min="1" max="1" width="22.5" customWidth="1"/>
+    <col min="2" max="2" width="56.5" customWidth="1"/>
+    <col min="3" max="3" width="26.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -4075,7 +4088,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.6">
+    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>4</v>
       </c>
@@ -4084,7 +4097,7 @@
       </c>
       <c r="C3" s="31"/>
     </row>
-    <row r="4" spans="1:3" ht="15.6">
+    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>7</v>
       </c>
@@ -4093,7 +4106,7 @@
       </c>
       <c r="C4" s="11"/>
     </row>
-    <row r="5" spans="1:3" ht="15.6">
+    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
         <v>9</v>
       </c>
@@ -4104,7 +4117,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.6">
+    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
         <v>11</v>
       </c>
@@ -4115,7 +4128,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.6">
+    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
         <v>13</v>
       </c>
@@ -4126,7 +4139,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.6">
+    <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
         <v>15</v>
       </c>
@@ -4137,7 +4150,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.6">
+    <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
         <v>17</v>
       </c>
@@ -4148,7 +4161,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.6">
+    <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
         <v>19</v>
       </c>
@@ -4159,7 +4172,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.6">
+    <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
         <v>21</v>
       </c>
@@ -4168,7 +4181,7 @@
       </c>
       <c r="C11" s="11"/>
     </row>
-    <row r="12" spans="1:3" ht="15.6">
+    <row r="12" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
         <v>23</v>
       </c>
@@ -4179,7 +4192,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.6">
+    <row r="13" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
         <v>25</v>
       </c>
@@ -4190,7 +4203,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15.6">
+    <row r="14" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
         <v>27</v>
       </c>
@@ -4201,7 +4214,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15.6">
+    <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
         <v>29</v>
       </c>
@@ -4212,7 +4225,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.6">
+    <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>31</v>
       </c>
@@ -4223,7 +4236,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15.6">
+    <row r="17" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
         <v>33</v>
       </c>
@@ -4234,7 +4247,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15.6">
+    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
         <v>35</v>
       </c>
@@ -4245,7 +4258,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.6">
+    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
         <v>37</v>
       </c>
@@ -4254,7 +4267,7 @@
       </c>
       <c r="C19" s="10"/>
     </row>
-    <row r="20" spans="1:3" ht="15.6">
+    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>39</v>
       </c>
@@ -4263,7 +4276,7 @@
       </c>
       <c r="C20" s="11"/>
     </row>
-    <row r="21" spans="1:3" ht="15.6">
+    <row r="21" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
         <v>41</v>
       </c>
@@ -4274,7 +4287,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15.6">
+    <row r="22" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
         <v>43</v>
       </c>
@@ -4285,7 +4298,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15.6">
+    <row r="23" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
         <v>45</v>
       </c>
@@ -4296,7 +4309,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15.6">
+    <row r="24" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
         <v>47</v>
       </c>
@@ -4307,7 +4320,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
         <v>49</v>
       </c>
@@ -4318,7 +4331,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15.6">
+    <row r="26" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
         <v>51</v>
       </c>
@@ -4342,15 +4355,15 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" style="17" customWidth="1"/>
-    <col min="2" max="2" width="45.21875" style="17" customWidth="1"/>
+    <col min="1" max="1" width="31.83203125" style="17" customWidth="1"/>
+    <col min="2" max="2" width="45.1640625" style="17" customWidth="1"/>
     <col min="3" max="3" width="49" style="17" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="17"/>
+    <col min="4" max="16384" width="8.83203125" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
@@ -4361,7 +4374,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
         <v>4</v>
       </c>
@@ -4372,7 +4385,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
         <v>7</v>
       </c>
@@ -4383,7 +4396,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>9</v>
       </c>
@@ -4394,7 +4407,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
         <v>11</v>
       </c>
@@ -4405,7 +4418,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
         <v>13</v>
       </c>
@@ -4416,7 +4429,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="22" t="s">
         <v>15</v>
       </c>
@@ -4427,7 +4440,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="22" t="s">
         <v>17</v>
       </c>
@@ -4438,7 +4451,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="22" t="s">
         <v>19</v>
       </c>
@@ -4449,7 +4462,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="34" t="s">
         <v>21</v>
       </c>
@@ -4458,7 +4471,7 @@
       </c>
       <c r="C10" s="34"/>
     </row>
-    <row r="11" spans="1:3" ht="15" customHeight="1">
+    <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="22" t="s">
         <v>23</v>
       </c>
@@ -4469,7 +4482,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="22" t="s">
         <v>25</v>
       </c>
@@ -4480,7 +4493,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="22" t="s">
         <v>27</v>
       </c>
@@ -4491,7 +4504,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="19.2" customHeight="1">
+    <row r="14" spans="1:3" ht="19.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>29</v>
       </c>
@@ -4502,7 +4515,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="19.8" customHeight="1">
+    <row r="15" spans="1:3" ht="19.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="s">
         <v>31</v>
       </c>
@@ -4513,7 +4526,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="17.399999999999999" customHeight="1">
+    <row r="16" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="22" t="s">
         <v>33</v>
       </c>
@@ -4524,7 +4537,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="16.8" customHeight="1">
+    <row r="17" spans="1:3" ht="16.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="16" t="s">
         <v>35</v>
       </c>
@@ -4535,7 +4548,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="16" t="s">
         <v>37</v>
       </c>
@@ -4546,7 +4559,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="34" t="s">
         <v>39</v>
       </c>
@@ -4555,7 +4568,7 @@
       </c>
       <c r="C19" s="34"/>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="22" t="s">
         <v>41</v>
       </c>
@@ -4566,7 +4579,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="22" t="s">
         <v>43</v>
       </c>
@@ -4577,7 +4590,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="22" t="s">
         <v>45</v>
       </c>
@@ -4588,7 +4601,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="22" t="s">
         <v>47</v>
       </c>
@@ -4599,7 +4612,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="22" t="s">
         <v>49</v>
       </c>
@@ -4623,15 +4636,15 @@
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.5546875" style="32" customWidth="1"/>
-    <col min="2" max="2" width="70.44140625" style="32" customWidth="1"/>
-    <col min="3" max="3" width="45.77734375" style="32" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="32"/>
+    <col min="1" max="1" width="21.5" style="32" customWidth="1"/>
+    <col min="2" max="2" width="70.5" style="32" customWidth="1"/>
+    <col min="3" max="3" width="45.83203125" style="32" customWidth="1"/>
+    <col min="4" max="16384" width="8.83203125" style="32"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
@@ -4642,7 +4655,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="37" t="s">
         <v>4</v>
       </c>
@@ -4651,7 +4664,7 @@
       </c>
       <c r="C2" s="37"/>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="37" t="s">
         <v>7</v>
       </c>
@@ -4660,7 +4673,7 @@
       </c>
       <c r="C3" s="37"/>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="37" t="s">
         <v>9</v>
       </c>
@@ -4669,7 +4682,7 @@
       </c>
       <c r="C4" s="37"/>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="37" t="s">
         <v>11</v>
       </c>
@@ -4678,7 +4691,7 @@
       </c>
       <c r="C5" s="37"/>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="37" t="s">
         <v>13</v>
       </c>
@@ -4687,7 +4700,7 @@
       </c>
       <c r="C6" s="37"/>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="37" t="s">
         <v>15</v>
       </c>
@@ -4696,7 +4709,7 @@
       </c>
       <c r="C7" s="37"/>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="37" t="s">
         <v>17</v>
       </c>
@@ -4705,7 +4718,7 @@
       </c>
       <c r="C8" s="37"/>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="37" t="s">
         <v>19</v>
       </c>
@@ -4714,7 +4727,7 @@
       </c>
       <c r="C9" s="37"/>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="37" t="s">
         <v>21</v>
       </c>
@@ -4723,7 +4736,7 @@
       </c>
       <c r="C10" s="37"/>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="37" t="s">
         <v>23</v>
       </c>
@@ -4732,7 +4745,7 @@
       </c>
       <c r="C11" s="37"/>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="37" t="s">
         <v>25</v>
       </c>
@@ -4741,7 +4754,7 @@
       </c>
       <c r="C12" s="37"/>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="37" t="s">
         <v>27</v>
       </c>
@@ -4750,7 +4763,7 @@
       </c>
       <c r="C13" s="37"/>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="37" t="s">
         <v>29</v>
       </c>
@@ -4759,7 +4772,7 @@
       </c>
       <c r="C14" s="37"/>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="37" t="s">
         <v>31</v>
       </c>
@@ -4768,7 +4781,7 @@
       </c>
       <c r="C15" s="37"/>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="22" t="s">
         <v>33</v>
       </c>
@@ -4779,7 +4792,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="37" t="s">
         <v>35</v>
       </c>
@@ -4788,7 +4801,7 @@
       </c>
       <c r="C17" s="37"/>
     </row>
-    <row r="18" spans="1:3" ht="15.6" customHeight="1">
+    <row r="18" spans="1:3" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="37" t="s">
         <v>37</v>
       </c>
@@ -4797,7 +4810,7 @@
       </c>
       <c r="C18" s="37"/>
     </row>
-    <row r="19" spans="1:3" ht="13.8" hidden="1" customHeight="1">
+    <row r="19" spans="1:3" ht="13.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="37" t="s">
         <v>39</v>
       </c>
@@ -4806,7 +4819,7 @@
       </c>
       <c r="C19" s="37"/>
     </row>
-    <row r="20" spans="1:3" ht="18" hidden="1" customHeight="1">
+    <row r="20" spans="1:3" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="37" t="s">
         <v>41</v>
       </c>
@@ -4815,7 +4828,7 @@
       </c>
       <c r="C20" s="37"/>
     </row>
-    <row r="21" spans="1:3" hidden="1">
+    <row r="21" spans="1:3" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="37" t="s">
         <v>43</v>
       </c>
@@ -4824,7 +4837,7 @@
       </c>
       <c r="C21" s="37"/>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="22" t="s">
         <v>45</v>
       </c>
@@ -4835,7 +4848,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="17.399999999999999" customHeight="1">
+    <row r="23" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="22" t="s">
         <v>47</v>
       </c>
@@ -4846,7 +4859,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="16.8" customHeight="1">
+    <row r="24" spans="1:3" ht="16.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="22" t="s">
         <v>49</v>
       </c>
@@ -4857,7 +4870,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="18" customHeight="1">
+    <row r="25" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="22" t="s">
         <v>51</v>
       </c>
@@ -4868,7 +4881,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="18.600000000000001" customHeight="1">
+    <row r="26" spans="1:3" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="37" t="s">
         <v>53</v>
       </c>
@@ -4877,7 +4890,7 @@
       </c>
       <c r="C26" s="37"/>
     </row>
-    <row r="27" spans="1:3" ht="15.6" customHeight="1">
+    <row r="27" spans="1:3" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="37" t="s">
         <v>55</v>
       </c>
@@ -4886,7 +4899,7 @@
       </c>
       <c r="C27" s="37"/>
     </row>
-    <row r="28" spans="1:3" ht="16.8" customHeight="1">
+    <row r="28" spans="1:3" ht="16.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="37" t="s">
         <v>57</v>
       </c>
@@ -4895,7 +4908,7 @@
       </c>
       <c r="C28" s="37"/>
     </row>
-    <row r="29" spans="1:3" ht="15.6" customHeight="1">
+    <row r="29" spans="1:3" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="37" t="s">
         <v>59</v>
       </c>
@@ -4904,7 +4917,7 @@
       </c>
       <c r="C29" s="37"/>
     </row>
-    <row r="30" spans="1:3" ht="15" customHeight="1">
+    <row r="30" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="37" t="s">
         <v>61</v>
       </c>
@@ -4913,7 +4926,7 @@
       </c>
       <c r="C30" s="37"/>
     </row>
-    <row r="31" spans="1:3" ht="15.6">
+    <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="22" t="s">
         <v>63</v>
       </c>
@@ -4924,7 +4937,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15.6">
+    <row r="32" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="22" t="s">
         <v>65</v>
       </c>
@@ -4935,7 +4948,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15.6">
+    <row r="33" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="22" t="s">
         <v>67</v>
       </c>
@@ -4946,7 +4959,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="22" t="s">
         <v>69</v>
       </c>
@@ -4957,7 +4970,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="22" t="s">
         <v>71</v>
       </c>
@@ -4979,19 +4992,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B222DBB3-E49F-4DB0-A9FD-74B741DD2ECD}">
   <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C4"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29.33203125" style="45" customWidth="1"/>
     <col min="2" max="2" width="67" style="45" customWidth="1"/>
-    <col min="3" max="3" width="28.5546875" style="45" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="45"/>
+    <col min="3" max="3" width="28.5" style="45" customWidth="1"/>
+    <col min="4" max="16384" width="8.83203125" style="45"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
@@ -5002,7 +5015,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="51" t="s">
         <v>4</v>
       </c>
@@ -5013,7 +5026,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="51" t="s">
         <v>7</v>
       </c>
@@ -5024,7 +5037,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="51" t="s">
         <v>9</v>
       </c>
@@ -5035,7 +5048,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="46" t="s">
         <v>11</v>
       </c>
@@ -5044,7 +5057,7 @@
       </c>
       <c r="C5" s="46"/>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="46" t="s">
         <v>13</v>
       </c>
@@ -5053,7 +5066,7 @@
       </c>
       <c r="C6" s="46"/>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="46" t="s">
         <v>15</v>
       </c>
@@ -5062,7 +5075,7 @@
       </c>
       <c r="C7" s="46"/>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="46" t="s">
         <v>17</v>
       </c>
@@ -5071,7 +5084,7 @@
       </c>
       <c r="C8" s="46"/>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="46" t="s">
         <v>19</v>
       </c>
@@ -5080,7 +5093,7 @@
       </c>
       <c r="C9" s="46"/>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="46" t="s">
         <v>21</v>
       </c>
@@ -5089,7 +5102,7 @@
       </c>
       <c r="C10" s="46"/>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="46" t="s">
         <v>23</v>
       </c>
@@ -5098,7 +5111,7 @@
       </c>
       <c r="C11" s="46"/>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="46" t="s">
         <v>25</v>
       </c>
@@ -5107,7 +5120,7 @@
       </c>
       <c r="C12" s="46"/>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="51" t="s">
         <v>27</v>
       </c>
@@ -5118,7 +5131,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="51" t="s">
         <v>29</v>
       </c>
@@ -5129,7 +5142,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="51" t="s">
         <v>31</v>
       </c>
@@ -5140,7 +5153,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="51" t="s">
         <v>33</v>
       </c>
@@ -5151,7 +5164,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="51" t="s">
         <v>35</v>
       </c>
@@ -5162,7 +5175,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="51" t="s">
         <v>37</v>
       </c>
@@ -5173,7 +5186,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="51" t="s">
         <v>39</v>
       </c>
@@ -5184,7 +5197,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="51" t="s">
         <v>41</v>
       </c>
@@ -5195,7 +5208,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="51" t="s">
         <v>43</v>
       </c>
@@ -5206,7 +5219,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="51" t="s">
         <v>45</v>
       </c>
@@ -5217,16 +5230,16 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="46" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="51" t="s">
         <v>47</v>
       </c>
-      <c r="B23" s="19" t="s">
+      <c r="B23" s="24" t="s">
         <v>330</v>
       </c>
-      <c r="C23" s="46"/>
-    </row>
-    <row r="24" spans="1:3">
+      <c r="C23" s="51"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="46" t="s">
         <v>49</v>
       </c>
@@ -5235,25 +5248,25 @@
       </c>
       <c r="C24" s="46"/>
     </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="46" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="51" t="s">
         <v>51</v>
       </c>
-      <c r="B25" s="19" t="s">
+      <c r="B25" s="24" t="s">
         <v>332</v>
       </c>
-      <c r="C25" s="46"/>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="46" t="s">
+      <c r="C25" s="51"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="B26" s="19" t="s">
+      <c r="B26" s="24" t="s">
         <v>333</v>
       </c>
-      <c r="C26" s="46"/>
-    </row>
-    <row r="27" spans="1:3">
+      <c r="C26" s="51"/>
+    </row>
+    <row r="27" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="46" t="s">
         <v>55</v>
       </c>
@@ -5262,7 +5275,7 @@
       </c>
       <c r="C27" s="46"/>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="46" t="s">
         <v>57</v>
       </c>
@@ -5271,7 +5284,7 @@
       </c>
       <c r="C28" s="46"/>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="46" t="s">
         <v>59</v>
       </c>
@@ -5280,7 +5293,7 @@
       </c>
       <c r="C29" s="46"/>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="46" t="s">
         <v>61</v>
       </c>
@@ -5289,7 +5302,7 @@
       </c>
       <c r="C30" s="46"/>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="51" t="s">
         <v>63</v>
       </c>
@@ -5300,7 +5313,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="51" t="s">
         <v>65</v>
       </c>
@@ -5311,7 +5324,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="51" t="s">
         <v>67</v>
       </c>
@@ -5322,7 +5335,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="51" t="s">
         <v>69</v>
       </c>
@@ -5333,7 +5346,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="46" t="s">
         <v>71</v>
       </c>
@@ -5342,7 +5355,7 @@
       </c>
       <c r="C35" s="46"/>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="51" t="s">
         <v>73</v>
       </c>
@@ -5353,7 +5366,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="46" t="s">
         <v>75</v>
       </c>
@@ -5362,7 +5375,7 @@
       </c>
       <c r="C37" s="46"/>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="51" t="s">
         <v>77</v>
       </c>
@@ -5373,7 +5386,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="51" t="s">
         <v>79</v>
       </c>
@@ -5384,7 +5397,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="51" t="s">
         <v>81</v>
       </c>
@@ -5395,7 +5408,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="51" t="s">
         <v>83</v>
       </c>
@@ -5406,7 +5419,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="51" t="s">
         <v>85</v>
       </c>
@@ -5417,7 +5430,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="51" t="s">
         <v>87</v>
       </c>
@@ -5428,7 +5441,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="51" t="s">
         <v>88</v>
       </c>
@@ -5439,16 +5452,16 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
-      <c r="A45" s="46" t="s">
+    <row r="45" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A45" s="51" t="s">
         <v>89</v>
       </c>
-      <c r="B45" s="21" t="s">
+      <c r="B45" s="23" t="s">
         <v>352</v>
       </c>
-      <c r="C45" s="46"/>
-    </row>
-    <row r="46" spans="1:3">
+      <c r="C45" s="51"/>
+    </row>
+    <row r="46" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="46" t="s">
         <v>90</v>
       </c>
@@ -5457,7 +5470,7 @@
       </c>
       <c r="C46" s="46"/>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="51" t="s">
         <v>92</v>
       </c>
@@ -5468,7 +5481,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="46" t="s">
         <v>94</v>
       </c>
@@ -5491,14 +5504,14 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
+    <col min="1" max="1" width="31.83203125" customWidth="1"/>
     <col min="2" max="2" width="60" customWidth="1"/>
-    <col min="3" max="3" width="41.88671875" customWidth="1"/>
+    <col min="3" max="3" width="41.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
@@ -5509,7 +5522,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="46" t="s">
         <v>4</v>
       </c>
@@ -5518,7 +5531,7 @@
       </c>
       <c r="C2" s="46"/>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="46" t="s">
         <v>7</v>
       </c>
@@ -5527,7 +5540,7 @@
       </c>
       <c r="C3" s="46"/>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="46" t="s">
         <v>9</v>
       </c>
@@ -5536,7 +5549,7 @@
       </c>
       <c r="C4" s="46"/>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="46" t="s">
         <v>11</v>
       </c>
@@ -5545,7 +5558,7 @@
       </c>
       <c r="C5" s="46"/>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="46" t="s">
         <v>13</v>
       </c>
@@ -5554,7 +5567,7 @@
       </c>
       <c r="C6" s="46"/>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="46" t="s">
         <v>15</v>
       </c>
@@ -5563,7 +5576,7 @@
       </c>
       <c r="C7" s="46"/>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="46" t="s">
         <v>17</v>
       </c>
@@ -5572,7 +5585,7 @@
       </c>
       <c r="C8" s="46"/>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="46" t="s">
         <v>19</v>
       </c>
@@ -5581,7 +5594,7 @@
       </c>
       <c r="C9" s="46"/>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="46" t="s">
         <v>21</v>
       </c>
@@ -5590,7 +5603,7 @@
       </c>
       <c r="C10" s="46"/>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="51" t="s">
         <v>23</v>
       </c>
@@ -5599,7 +5612,7 @@
       </c>
       <c r="C11" s="51"/>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="46" t="s">
         <v>25</v>
       </c>
@@ -5608,7 +5621,7 @@
       </c>
       <c r="C12" s="46"/>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="46" t="s">
         <v>27</v>
       </c>
@@ -5617,7 +5630,7 @@
       </c>
       <c r="C13" s="46"/>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="46" t="s">
         <v>29</v>
       </c>
@@ -5626,7 +5639,7 @@
       </c>
       <c r="C14" s="46"/>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="46" t="s">
         <v>31</v>
       </c>
@@ -5635,7 +5648,7 @@
       </c>
       <c r="C15" s="46"/>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="46" t="s">
         <v>33</v>
       </c>
@@ -5644,7 +5657,7 @@
       </c>
       <c r="C16" s="46"/>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="46" t="s">
         <v>35</v>
       </c>
@@ -5653,7 +5666,7 @@
       </c>
       <c r="C17" s="46"/>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="46" t="s">
         <v>37</v>
       </c>
@@ -5662,7 +5675,7 @@
       </c>
       <c r="C18" s="46"/>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="46" t="s">
         <v>39</v>
       </c>
@@ -5671,7 +5684,7 @@
       </c>
       <c r="C19" s="46"/>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="46" t="s">
         <v>41</v>
       </c>
@@ -5680,7 +5693,7 @@
       </c>
       <c r="C20" s="46"/>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="46" t="s">
         <v>43</v>
       </c>
@@ -5689,7 +5702,7 @@
       </c>
       <c r="C21" s="46"/>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="46" t="s">
         <v>45</v>
       </c>
@@ -5712,14 +5725,14 @@
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.44140625" customWidth="1"/>
+    <col min="1" max="1" width="24.5" customWidth="1"/>
     <col min="2" max="2" width="32.6640625" customWidth="1"/>
-    <col min="3" max="3" width="71.44140625" customWidth="1"/>
+    <col min="3" max="3" width="71.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="47" t="s">
         <v>398</v>
       </c>
@@ -5733,7 +5746,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="48" t="s">
         <v>377</v>
       </c>
@@ -5745,7 +5758,7 @@
       </c>
       <c r="D2" s="50"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="48" t="s">
         <v>377</v>
       </c>
@@ -5757,7 +5770,7 @@
       </c>
       <c r="D3" s="50"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="48" t="s">
         <v>377</v>
       </c>
@@ -5769,7 +5782,7 @@
       </c>
       <c r="D4" s="50"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="48" t="s">
         <v>377</v>
       </c>
@@ -5781,7 +5794,7 @@
       </c>
       <c r="D5" s="50"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="48" t="s">
         <v>377</v>
       </c>
@@ -5793,7 +5806,7 @@
       </c>
       <c r="D6" s="50"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="48" t="s">
         <v>377</v>
       </c>
@@ -5805,7 +5818,7 @@
       </c>
       <c r="D7" s="50"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="48" t="s">
         <v>377</v>
       </c>
@@ -5817,7 +5830,7 @@
       </c>
       <c r="D8" s="50"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="48" t="s">
         <v>377</v>
       </c>
@@ -5829,7 +5842,7 @@
       </c>
       <c r="D9" s="50"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="48" t="s">
         <v>377</v>
       </c>
@@ -5841,7 +5854,7 @@
       </c>
       <c r="D10" s="50"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="48" t="s">
         <v>377</v>
       </c>

</xml_diff>